<commit_message>
Auto-committed on 2023/05/24 週三 11:57:14.22
</commit_message>
<xml_diff>
--- a/Program/Other/LP005_底稿_協辦考核核算.xlsx
+++ b/Program/Other/LP005_底稿_協辦考核核算.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SKL\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SVN\iTX\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D0C2328-2CC3-4542-A4DC-C88D40A139C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52F485CE-8C0B-41B7-9B93-5F2B325BC3EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="791" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" tabRatio="791" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1月件數" sheetId="70" r:id="rId1"/>
@@ -787,7 +787,7 @@
       <charset val="136"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -796,31 +796,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="41"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFEAEAEA"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -861,7 +837,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -871,38 +847,113 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="10" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -913,80 +964,14 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="4" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="3" fillId="4" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="6" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="6" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="4" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="10" fillId="4" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1780,50 +1765,50 @@
   <sheetPr codeName="工作表1"/>
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18.6640625" defaultRowHeight="16.2"/>
+  <sheetFormatPr defaultColWidth="18.6328125" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" style="11" customWidth="1"/>
-    <col min="3" max="3" width="16.21875" style="11" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" style="11" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" style="11" customWidth="1"/>
-    <col min="6" max="6" width="15" style="11" customWidth="1"/>
-    <col min="7" max="7" width="16.88671875" style="11" customWidth="1"/>
-    <col min="8" max="8" width="15.77734375" style="11" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" style="11" customWidth="1"/>
-    <col min="10" max="16384" width="18.6640625" style="11"/>
+    <col min="1" max="1" width="10.453125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6328125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="16.1796875" style="7" customWidth="1"/>
+    <col min="4" max="4" width="18.36328125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="11.90625" style="7" customWidth="1"/>
+    <col min="6" max="6" width="15" style="7" customWidth="1"/>
+    <col min="7" max="7" width="16.90625" style="7" customWidth="1"/>
+    <col min="8" max="8" width="15.81640625" style="7" customWidth="1"/>
+    <col min="9" max="9" width="13.36328125" style="7" customWidth="1"/>
+    <col min="10" max="16384" width="18.6328125" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="6" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1839,280 +1824,449 @@
   <sheetPr codeName="Sheet8">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P8"/>
+  <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="N17" sqref="A1:O17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="9.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.44140625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="8.109375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="9" style="4"/>
-    <col min="5" max="5" width="8.33203125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="6.6640625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="8.109375" style="5" customWidth="1"/>
-    <col min="8" max="8" width="6.6640625" style="5" customWidth="1"/>
-    <col min="9" max="9" width="8.109375" style="5" customWidth="1"/>
-    <col min="10" max="10" width="6.6640625" style="5" customWidth="1"/>
-    <col min="11" max="11" width="8.109375" style="5" customWidth="1"/>
-    <col min="12" max="12" width="7.109375" style="6" customWidth="1"/>
-    <col min="13" max="13" width="8.109375" style="5" customWidth="1"/>
-    <col min="14" max="14" width="10" style="4" customWidth="1"/>
-    <col min="15" max="15" width="8.109375" style="7" customWidth="1"/>
-    <col min="16" max="16" width="7.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.453125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.08984375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9" style="1"/>
+    <col min="5" max="5" width="8.36328125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="6.6328125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="8.08984375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="6.6328125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="8.08984375" style="3" customWidth="1"/>
+    <col min="10" max="10" width="6.6328125" style="3" customWidth="1"/>
+    <col min="11" max="11" width="8.08984375" style="3" customWidth="1"/>
+    <col min="12" max="12" width="7.08984375" style="4" customWidth="1"/>
+    <col min="13" max="13" width="8.08984375" style="3" customWidth="1"/>
+    <col min="14" max="14" width="10" style="1" customWidth="1"/>
+    <col min="15" max="15" width="8.08984375" style="5" customWidth="1"/>
+    <col min="16" max="16" width="7.90625" style="1" customWidth="1"/>
     <col min="17" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="18">
-      <c r="A1" s="37" t="s">
+    <row r="1" spans="1:15" ht="18.5">
+      <c r="A1" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
-    </row>
-    <row r="2" spans="1:16" ht="16.5" customHeight="1">
-      <c r="A2" s="39" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="39" t="s">
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+    </row>
+    <row r="2" spans="1:15" ht="16.5" customHeight="1">
+      <c r="A2" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="39" t="s">
+      <c r="D2" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="40" t="s">
+      <c r="E2" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="31" t="s">
+      <c r="F2" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31" t="s">
+      <c r="G2" s="20"/>
+      <c r="H2" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31" t="s">
+      <c r="I2" s="20"/>
+      <c r="J2" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31" t="s">
+      <c r="K2" s="20"/>
+      <c r="L2" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="M2" s="31"/>
-      <c r="N2" s="30" t="s">
+      <c r="M2" s="20"/>
+      <c r="N2" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="O2" s="38" t="s">
+      <c r="O2" s="22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:16" s="2" customFormat="1">
-      <c r="A3" s="39"/>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="20" t="s">
+    <row r="3" spans="1:15" s="2" customFormat="1">
+      <c r="A3" s="18"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="20" t="s">
+      <c r="H3" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="20" t="s">
+      <c r="I3" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="20" t="s">
+      <c r="J3" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="20" t="s">
+      <c r="K3" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="20" t="s">
+      <c r="L3" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="M3" s="20" t="s">
+      <c r="M3" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="30"/>
-      <c r="O3" s="30"/>
-    </row>
-    <row r="4" spans="1:16">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="22"/>
-      <c r="L4" s="23"/>
-      <c r="M4" s="22"/>
-      <c r="N4" s="24"/>
-      <c r="O4" s="9"/>
-      <c r="P4" s="3"/>
-    </row>
-    <row r="5" spans="1:16">
-      <c r="A5" s="33" t="s">
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" s="25"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="28"/>
+      <c r="L4" s="29"/>
+      <c r="M4" s="28"/>
+      <c r="N4" s="30"/>
+      <c r="O4" s="26"/>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="33"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="25">
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="29">
         <f t="shared" ref="F5:K5" si="0">SUM(F4:F4)</f>
         <v>0</v>
       </c>
-      <c r="G5" s="25">
+      <c r="G5" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H5" s="25">
+      <c r="H5" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I5" s="26">
+      <c r="I5" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J5" s="25">
+      <c r="J5" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K5" s="25">
+      <c r="K5" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L5" s="25">
+      <c r="L5" s="29">
         <f>F5+H5+J5</f>
         <v>0</v>
       </c>
-      <c r="M5" s="26">
+      <c r="M5" s="28">
         <f>G5+I5+K5</f>
         <v>0</v>
       </c>
-      <c r="N5" s="27"/>
-      <c r="O5" s="28"/>
-    </row>
-    <row r="6" spans="1:16">
-      <c r="A6" s="33" t="s">
+      <c r="N5" s="25"/>
+      <c r="O5" s="31"/>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="33"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="35">
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="20">
         <f>SUBTOTAL(3,$C4:$C4)</f>
         <v>0</v>
       </c>
-      <c r="G6" s="35"/>
-      <c r="H6" s="36">
+      <c r="G6" s="20"/>
+      <c r="H6" s="32">
         <f>SUBTOTAL(3,$C4:$C4)</f>
         <v>0</v>
       </c>
-      <c r="I6" s="36"/>
-      <c r="J6" s="35">
+      <c r="I6" s="32"/>
+      <c r="J6" s="20">
         <f>SUBTOTAL(3,$C4:$C4)</f>
         <v>0</v>
       </c>
-      <c r="K6" s="35"/>
-      <c r="L6" s="35">
+      <c r="K6" s="20"/>
+      <c r="L6" s="20">
         <f>SUBTOTAL(3,$C4:$C4)</f>
         <v>0</v>
       </c>
-      <c r="M6" s="35"/>
-      <c r="N6" s="27"/>
-      <c r="O6" s="28"/>
-    </row>
-    <row r="7" spans="1:16">
-      <c r="A7" s="41" t="s">
+      <c r="M6" s="20"/>
+      <c r="N6" s="25"/>
+      <c r="O6" s="31"/>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="41"/>
-      <c r="C7" s="41"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="32">
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="20">
         <f>COUNTIF(F4:F4,"&lt;&gt;0")</f>
         <v>1</v>
       </c>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32">
+      <c r="G7" s="20"/>
+      <c r="H7" s="20">
         <f>COUNTIF(H4:H4,"&lt;&gt;0")</f>
         <v>1</v>
       </c>
-      <c r="I7" s="32"/>
-      <c r="J7" s="32">
+      <c r="I7" s="20"/>
+      <c r="J7" s="20">
         <f>COUNTIF(J4:J4,"&lt;&gt;0")</f>
         <v>1</v>
       </c>
-      <c r="K7" s="32"/>
-      <c r="L7" s="32">
+      <c r="K7" s="20"/>
+      <c r="L7" s="20">
         <f>COUNTIF(L4:L4,"&lt;&gt;0")</f>
         <v>1</v>
       </c>
-      <c r="M7" s="32"/>
-      <c r="N7" s="32"/>
-      <c r="O7" s="32"/>
-    </row>
-    <row r="8" spans="1:16">
-      <c r="A8" s="41" t="s">
+      <c r="M7" s="20"/>
+      <c r="N7" s="20"/>
+      <c r="O7" s="20"/>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="41"/>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="34" t="e">
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="33" t="e">
         <f>F7/F6</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34" t="e">
+      <c r="G8" s="33"/>
+      <c r="H8" s="33" t="e">
         <f>H7/H6</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I8" s="34"/>
-      <c r="J8" s="34" t="e">
+      <c r="I8" s="33"/>
+      <c r="J8" s="33" t="e">
         <f>J7/J6</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K8" s="34"/>
-      <c r="L8" s="34" t="e">
+      <c r="K8" s="33"/>
+      <c r="L8" s="33" t="e">
         <f>L7/L6</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M8" s="34"/>
-      <c r="N8" s="32"/>
-      <c r="O8" s="32"/>
+      <c r="M8" s="33"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="20"/>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" s="17"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="34"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="34"/>
+      <c r="I9" s="34"/>
+      <c r="J9" s="34"/>
+      <c r="K9" s="34"/>
+      <c r="L9" s="35"/>
+      <c r="M9" s="34"/>
+      <c r="N9" s="17"/>
+      <c r="O9" s="36"/>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" s="17"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="34"/>
+      <c r="I10" s="34"/>
+      <c r="J10" s="34"/>
+      <c r="K10" s="34"/>
+      <c r="L10" s="35"/>
+      <c r="M10" s="34"/>
+      <c r="N10" s="17"/>
+      <c r="O10" s="36"/>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" s="17"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="34"/>
+      <c r="J11" s="34"/>
+      <c r="K11" s="34"/>
+      <c r="L11" s="35"/>
+      <c r="M11" s="34"/>
+      <c r="N11" s="17"/>
+      <c r="O11" s="36"/>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" s="17"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
+      <c r="J12" s="34"/>
+      <c r="K12" s="34"/>
+      <c r="L12" s="35"/>
+      <c r="M12" s="34"/>
+      <c r="N12" s="17"/>
+      <c r="O12" s="36"/>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" s="17"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="34"/>
+      <c r="I13" s="34"/>
+      <c r="J13" s="34"/>
+      <c r="K13" s="34"/>
+      <c r="L13" s="35"/>
+      <c r="M13" s="34"/>
+      <c r="N13" s="17"/>
+      <c r="O13" s="36"/>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" s="17"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="34"/>
+      <c r="K14" s="34"/>
+      <c r="L14" s="35"/>
+      <c r="M14" s="34"/>
+      <c r="N14" s="17"/>
+      <c r="O14" s="36"/>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15" s="17"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="34"/>
+      <c r="I15" s="34"/>
+      <c r="J15" s="34"/>
+      <c r="K15" s="34"/>
+      <c r="L15" s="35"/>
+      <c r="M15" s="34"/>
+      <c r="N15" s="17"/>
+      <c r="O15" s="36"/>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="A16" s="17"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="34"/>
+      <c r="J16" s="34"/>
+      <c r="K16" s="34"/>
+      <c r="L16" s="35"/>
+      <c r="M16" s="34"/>
+      <c r="N16" s="17"/>
+      <c r="O16" s="36"/>
+    </row>
+    <row r="17" spans="1:15">
+      <c r="A17" s="17"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="34"/>
+      <c r="H17" s="34"/>
+      <c r="I17" s="34"/>
+      <c r="J17" s="34"/>
+      <c r="K17" s="34"/>
+      <c r="L17" s="35"/>
+      <c r="M17" s="34"/>
+      <c r="N17" s="17"/>
+      <c r="O17" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="O2:O3"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:K6"/>
     <mergeCell ref="L6:M6"/>
     <mergeCell ref="N8:O8"/>
     <mergeCell ref="A7:E7"/>
@@ -2126,23 +2280,6 @@
     <mergeCell ref="H8:I8"/>
     <mergeCell ref="J8:K8"/>
     <mergeCell ref="L8:M8"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="A1:O1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="O2:O3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="O4">
@@ -2179,280 +2316,466 @@
   <sheetPr codeName="Sheet9">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P8"/>
+  <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="P17" sqref="A1:P17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="9.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.44140625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="8.109375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="9" style="4"/>
-    <col min="5" max="5" width="8.33203125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="6.6640625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="8.109375" style="5" customWidth="1"/>
-    <col min="8" max="8" width="6.6640625" style="5" customWidth="1"/>
-    <col min="9" max="9" width="8.109375" style="5" customWidth="1"/>
-    <col min="10" max="10" width="6.6640625" style="5" customWidth="1"/>
-    <col min="11" max="11" width="8.109375" style="5" customWidth="1"/>
-    <col min="12" max="12" width="7.109375" style="6" customWidth="1"/>
-    <col min="13" max="13" width="8.109375" style="5" customWidth="1"/>
-    <col min="14" max="14" width="10" style="4" customWidth="1"/>
-    <col min="15" max="15" width="8.109375" style="7" customWidth="1"/>
-    <col min="16" max="16" width="7.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.453125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.08984375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9" style="1"/>
+    <col min="5" max="5" width="8.36328125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="6.6328125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="8.08984375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="6.6328125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="8.08984375" style="3" customWidth="1"/>
+    <col min="10" max="10" width="6.6328125" style="3" customWidth="1"/>
+    <col min="11" max="11" width="8.08984375" style="3" customWidth="1"/>
+    <col min="12" max="12" width="7.08984375" style="4" customWidth="1"/>
+    <col min="13" max="13" width="8.08984375" style="3" customWidth="1"/>
+    <col min="14" max="14" width="10" style="1" customWidth="1"/>
+    <col min="15" max="15" width="8.08984375" style="5" customWidth="1"/>
+    <col min="16" max="16" width="7.90625" style="1" customWidth="1"/>
     <col min="17" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="18">
-      <c r="A1" s="37" t="s">
+    <row r="1" spans="1:16" ht="18.5">
+      <c r="A1" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="17"/>
     </row>
     <row r="2" spans="1:16" ht="16.5" customHeight="1">
-      <c r="A2" s="39" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="39" t="s">
+      <c r="A2" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="39" t="s">
+      <c r="D2" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="40" t="s">
+      <c r="E2" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="31" t="s">
+      <c r="F2" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31" t="s">
+      <c r="G2" s="20"/>
+      <c r="H2" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31" t="s">
+      <c r="I2" s="20"/>
+      <c r="J2" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31" t="s">
+      <c r="K2" s="20"/>
+      <c r="L2" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="M2" s="31"/>
-      <c r="N2" s="30" t="s">
+      <c r="M2" s="20"/>
+      <c r="N2" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="O2" s="38" t="s">
+      <c r="O2" s="22" t="s">
         <v>21</v>
       </c>
+      <c r="P2" s="17"/>
     </row>
     <row r="3" spans="1:16" s="2" customFormat="1">
-      <c r="A3" s="39"/>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="20" t="s">
+      <c r="A3" s="18"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="20" t="s">
+      <c r="H3" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="20" t="s">
+      <c r="I3" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="20" t="s">
+      <c r="J3" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="20" t="s">
+      <c r="K3" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="20" t="s">
+      <c r="L3" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="M3" s="20" t="s">
+      <c r="M3" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="30"/>
-      <c r="O3" s="30"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="24"/>
     </row>
     <row r="4" spans="1:16">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="22"/>
-      <c r="L4" s="23"/>
-      <c r="M4" s="22"/>
-      <c r="N4" s="24"/>
-      <c r="O4" s="9"/>
-      <c r="P4" s="3"/>
+      <c r="A4" s="25"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="28"/>
+      <c r="L4" s="29"/>
+      <c r="M4" s="28"/>
+      <c r="N4" s="30"/>
+      <c r="O4" s="26"/>
+      <c r="P4" s="17"/>
     </row>
     <row r="5" spans="1:16">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="33"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="25">
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="29">
         <f t="shared" ref="F5:K5" si="0">SUM(F4:F4)</f>
         <v>0</v>
       </c>
-      <c r="G5" s="25">
+      <c r="G5" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H5" s="25">
+      <c r="H5" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I5" s="26">
+      <c r="I5" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J5" s="25">
+      <c r="J5" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K5" s="25">
+      <c r="K5" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L5" s="25">
+      <c r="L5" s="29">
         <f>F5+H5+J5</f>
         <v>0</v>
       </c>
-      <c r="M5" s="26">
+      <c r="M5" s="28">
         <f>G5+I5+K5</f>
         <v>0</v>
       </c>
-      <c r="N5" s="27"/>
-      <c r="O5" s="28"/>
+      <c r="N5" s="25"/>
+      <c r="O5" s="31"/>
+      <c r="P5" s="17"/>
     </row>
     <row r="6" spans="1:16">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="33"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="35">
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="20">
         <f>SUBTOTAL(3,$C4:$C4)</f>
         <v>0</v>
       </c>
-      <c r="G6" s="35"/>
-      <c r="H6" s="36">
+      <c r="G6" s="20"/>
+      <c r="H6" s="32">
         <f>SUBTOTAL(3,$C4:$C4)</f>
         <v>0</v>
       </c>
-      <c r="I6" s="36"/>
-      <c r="J6" s="35">
+      <c r="I6" s="32"/>
+      <c r="J6" s="20">
         <f>SUBTOTAL(3,$C4:$C4)</f>
         <v>0</v>
       </c>
-      <c r="K6" s="35"/>
-      <c r="L6" s="35">
+      <c r="K6" s="20"/>
+      <c r="L6" s="20">
         <f>SUBTOTAL(3,$C4:$C4)</f>
         <v>0</v>
       </c>
-      <c r="M6" s="35"/>
-      <c r="N6" s="27"/>
-      <c r="O6" s="28"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="25"/>
+      <c r="O6" s="31"/>
+      <c r="P6" s="17"/>
     </row>
     <row r="7" spans="1:16">
-      <c r="A7" s="41" t="s">
+      <c r="A7" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="41"/>
-      <c r="C7" s="41"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="32">
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="20">
         <f>COUNTIF(F4:F4,"&lt;&gt;0")</f>
         <v>1</v>
       </c>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32">
+      <c r="G7" s="20"/>
+      <c r="H7" s="20">
         <f>COUNTIF(H4:H4,"&lt;&gt;0")</f>
         <v>1</v>
       </c>
-      <c r="I7" s="32"/>
-      <c r="J7" s="32">
+      <c r="I7" s="20"/>
+      <c r="J7" s="20">
         <f>COUNTIF(J4:J4,"&lt;&gt;0")</f>
         <v>1</v>
       </c>
-      <c r="K7" s="32"/>
-      <c r="L7" s="32">
+      <c r="K7" s="20"/>
+      <c r="L7" s="20">
         <f>COUNTIF(L4:L4,"&lt;&gt;0")</f>
         <v>1</v>
       </c>
-      <c r="M7" s="32"/>
-      <c r="N7" s="32"/>
-      <c r="O7" s="32"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="20"/>
+      <c r="O7" s="20"/>
+      <c r="P7" s="17"/>
     </row>
     <row r="8" spans="1:16">
-      <c r="A8" s="41" t="s">
+      <c r="A8" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="41"/>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="34" t="e">
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="33" t="e">
         <f>F7/F6</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34" t="e">
+      <c r="G8" s="33"/>
+      <c r="H8" s="33" t="e">
         <f>H7/H6</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I8" s="34"/>
-      <c r="J8" s="34" t="e">
+      <c r="I8" s="33"/>
+      <c r="J8" s="33" t="e">
         <f>J7/J6</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K8" s="34"/>
-      <c r="L8" s="34" t="e">
+      <c r="K8" s="33"/>
+      <c r="L8" s="33" t="e">
         <f>L7/L6</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M8" s="34"/>
-      <c r="N8" s="32"/>
-      <c r="O8" s="32"/>
+      <c r="M8" s="33"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="20"/>
+      <c r="P8" s="17"/>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="A9" s="17"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="34"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="34"/>
+      <c r="I9" s="34"/>
+      <c r="J9" s="34"/>
+      <c r="K9" s="34"/>
+      <c r="L9" s="35"/>
+      <c r="M9" s="34"/>
+      <c r="N9" s="17"/>
+      <c r="O9" s="36"/>
+      <c r="P9" s="17"/>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10" s="17"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="34"/>
+      <c r="I10" s="34"/>
+      <c r="J10" s="34"/>
+      <c r="K10" s="34"/>
+      <c r="L10" s="35"/>
+      <c r="M10" s="34"/>
+      <c r="N10" s="17"/>
+      <c r="O10" s="36"/>
+      <c r="P10" s="17"/>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11" s="17"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="34"/>
+      <c r="J11" s="34"/>
+      <c r="K11" s="34"/>
+      <c r="L11" s="35"/>
+      <c r="M11" s="34"/>
+      <c r="N11" s="17"/>
+      <c r="O11" s="36"/>
+      <c r="P11" s="17"/>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="A12" s="17"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
+      <c r="J12" s="34"/>
+      <c r="K12" s="34"/>
+      <c r="L12" s="35"/>
+      <c r="M12" s="34"/>
+      <c r="N12" s="17"/>
+      <c r="O12" s="36"/>
+      <c r="P12" s="17"/>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13" s="17"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="34"/>
+      <c r="I13" s="34"/>
+      <c r="J13" s="34"/>
+      <c r="K13" s="34"/>
+      <c r="L13" s="35"/>
+      <c r="M13" s="34"/>
+      <c r="N13" s="17"/>
+      <c r="O13" s="36"/>
+      <c r="P13" s="17"/>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="A14" s="17"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="34"/>
+      <c r="K14" s="34"/>
+      <c r="L14" s="35"/>
+      <c r="M14" s="34"/>
+      <c r="N14" s="17"/>
+      <c r="O14" s="36"/>
+      <c r="P14" s="17"/>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="A15" s="17"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="34"/>
+      <c r="I15" s="34"/>
+      <c r="J15" s="34"/>
+      <c r="K15" s="34"/>
+      <c r="L15" s="35"/>
+      <c r="M15" s="34"/>
+      <c r="N15" s="17"/>
+      <c r="O15" s="36"/>
+      <c r="P15" s="17"/>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="A16" s="17"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="34"/>
+      <c r="J16" s="34"/>
+      <c r="K16" s="34"/>
+      <c r="L16" s="35"/>
+      <c r="M16" s="34"/>
+      <c r="N16" s="17"/>
+      <c r="O16" s="36"/>
+      <c r="P16" s="17"/>
+    </row>
+    <row r="17" spans="1:16">
+      <c r="A17" s="17"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="34"/>
+      <c r="H17" s="34"/>
+      <c r="I17" s="34"/>
+      <c r="J17" s="34"/>
+      <c r="K17" s="34"/>
+      <c r="L17" s="35"/>
+      <c r="M17" s="34"/>
+      <c r="N17" s="17"/>
+      <c r="O17" s="36"/>
+      <c r="P17" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="O2:O3"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:K6"/>
     <mergeCell ref="L6:M6"/>
     <mergeCell ref="N8:O8"/>
     <mergeCell ref="A7:E7"/>
@@ -2466,23 +2789,6 @@
     <mergeCell ref="H8:I8"/>
     <mergeCell ref="J8:K8"/>
     <mergeCell ref="L8:M8"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="A1:O1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="O2:O3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="O4">
@@ -2519,89 +2825,213 @@
   <sheetPr codeName="工作表5">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:I4"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J14" sqref="A1:J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="8.33203125" style="17" customWidth="1"/>
-    <col min="2" max="2" width="15.77734375" style="18" customWidth="1"/>
-    <col min="3" max="3" width="15.5546875" style="18" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" style="18" customWidth="1"/>
-    <col min="5" max="5" width="16.109375" style="18" customWidth="1"/>
-    <col min="6" max="6" width="14.77734375" style="18" customWidth="1"/>
-    <col min="7" max="8" width="12.88671875" style="18" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" style="19" customWidth="1"/>
-    <col min="10" max="10" width="9" style="12"/>
-    <col min="11" max="16384" width="9" style="13"/>
+    <col min="1" max="1" width="8.36328125" style="13" customWidth="1"/>
+    <col min="2" max="2" width="15.81640625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="15.54296875" style="9" customWidth="1"/>
+    <col min="4" max="4" width="11.90625" style="9" customWidth="1"/>
+    <col min="5" max="5" width="16.08984375" style="9" customWidth="1"/>
+    <col min="6" max="6" width="14.81640625" style="9" customWidth="1"/>
+    <col min="7" max="8" width="12.90625" style="9" customWidth="1"/>
+    <col min="9" max="9" width="11.6328125" style="14" customWidth="1"/>
+    <col min="10" max="10" width="9" style="8"/>
+    <col min="11" max="16384" width="9" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="24.75" customHeight="1">
-      <c r="A1" s="29" t="s">
+    <row r="1" spans="1:10" ht="24.75" customHeight="1">
+      <c r="A1" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-    </row>
-    <row r="2" spans="1:9" ht="24" customHeight="1">
-      <c r="A2" s="14" t="s">
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="38"/>
+    </row>
+    <row r="2" spans="1:10" ht="24" customHeight="1">
+      <c r="A2" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="H2" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="I2" s="39" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="18.899999999999999" customHeight="1">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="16"/>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="14"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="16"/>
+      <c r="J2" s="38"/>
+    </row>
+    <row r="3" spans="1:10" ht="18.899999999999999" customHeight="1">
+      <c r="A3" s="39"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="38"/>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="39"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="41"/>
+      <c r="J4" s="38"/>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="42"/>
+      <c r="B5" s="43"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="44"/>
+      <c r="J5" s="38"/>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="42"/>
+      <c r="B6" s="43"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="44"/>
+      <c r="J6" s="38"/>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="42"/>
+      <c r="B7" s="43"/>
+      <c r="C7" s="43"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="44"/>
+      <c r="J7" s="38"/>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="42"/>
+      <c r="B8" s="43"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="44"/>
+      <c r="J8" s="38"/>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="42"/>
+      <c r="B9" s="43"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="43"/>
+      <c r="I9" s="44"/>
+      <c r="J9" s="38"/>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="42"/>
+      <c r="B10" s="43"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="43"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="44"/>
+      <c r="J10" s="38"/>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="42"/>
+      <c r="B11" s="43"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="44"/>
+      <c r="J11" s="38"/>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="42"/>
+      <c r="B12" s="43"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="43"/>
+      <c r="I12" s="44"/>
+      <c r="J12" s="38"/>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="42"/>
+      <c r="B13" s="43"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="44"/>
+      <c r="J13" s="38"/>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="42"/>
+      <c r="B14" s="43"/>
+      <c r="C14" s="43"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="43"/>
+      <c r="H14" s="43"/>
+      <c r="I14" s="44"/>
+      <c r="J14" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2691,45 +3121,45 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18.6640625" defaultRowHeight="16.2"/>
+  <sheetFormatPr defaultColWidth="18.6328125" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" style="11" customWidth="1"/>
-    <col min="2" max="2" width="6" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.21875" style="11" customWidth="1"/>
-    <col min="4" max="5" width="10.44140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15" style="11" customWidth="1"/>
-    <col min="7" max="7" width="16.88671875" style="11" customWidth="1"/>
-    <col min="8" max="8" width="15.77734375" style="11" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" style="11" customWidth="1"/>
-    <col min="10" max="16384" width="18.6640625" style="11"/>
+    <col min="1" max="1" width="13.90625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="6" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.1796875" style="7" customWidth="1"/>
+    <col min="4" max="5" width="10.453125" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" style="7" customWidth="1"/>
+    <col min="7" max="7" width="16.90625" style="7" customWidth="1"/>
+    <col min="8" max="8" width="15.81640625" style="7" customWidth="1"/>
+    <col min="9" max="9" width="13.36328125" style="7" customWidth="1"/>
+    <col min="10" max="16384" width="18.6328125" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="6" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2749,46 +3179,46 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18.6640625" defaultRowHeight="16.2"/>
+  <sheetFormatPr defaultColWidth="18.6328125" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" style="11" customWidth="1"/>
-    <col min="3" max="3" width="16.21875" style="11" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" style="11" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" style="11" customWidth="1"/>
-    <col min="6" max="6" width="15" style="11" customWidth="1"/>
-    <col min="7" max="7" width="16.88671875" style="11" customWidth="1"/>
-    <col min="8" max="8" width="15.77734375" style="11" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" style="11" customWidth="1"/>
-    <col min="10" max="16384" width="18.6640625" style="11"/>
+    <col min="1" max="1" width="10.453125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6328125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="16.1796875" style="7" customWidth="1"/>
+    <col min="4" max="4" width="18.36328125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="11.90625" style="7" customWidth="1"/>
+    <col min="6" max="6" width="15" style="7" customWidth="1"/>
+    <col min="7" max="7" width="16.90625" style="7" customWidth="1"/>
+    <col min="8" max="8" width="15.81640625" style="7" customWidth="1"/>
+    <col min="9" max="9" width="13.36328125" style="7" customWidth="1"/>
+    <col min="10" max="16384" width="18.6328125" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="6" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2807,45 +3237,45 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18.6640625" defaultRowHeight="16.2"/>
+  <sheetFormatPr defaultColWidth="18.6328125" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" style="11" customWidth="1"/>
-    <col min="2" max="2" width="6" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.21875" style="11" customWidth="1"/>
-    <col min="4" max="5" width="10.44140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15" style="11" customWidth="1"/>
-    <col min="7" max="7" width="16.88671875" style="11" customWidth="1"/>
-    <col min="8" max="8" width="15.77734375" style="11" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" style="11" customWidth="1"/>
-    <col min="10" max="16384" width="18.6640625" style="11"/>
+    <col min="1" max="1" width="13.90625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="6" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.1796875" style="7" customWidth="1"/>
+    <col min="4" max="5" width="10.453125" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" style="7" customWidth="1"/>
+    <col min="7" max="7" width="16.90625" style="7" customWidth="1"/>
+    <col min="8" max="8" width="15.81640625" style="7" customWidth="1"/>
+    <col min="9" max="9" width="13.36328125" style="7" customWidth="1"/>
+    <col min="10" max="16384" width="18.6328125" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="6" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2863,46 +3293,46 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18.6640625" defaultRowHeight="16.2"/>
+  <sheetFormatPr defaultColWidth="18.6328125" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" style="11" customWidth="1"/>
-    <col min="3" max="3" width="16.21875" style="11" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" style="11" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" style="11" customWidth="1"/>
-    <col min="6" max="6" width="15" style="11" customWidth="1"/>
-    <col min="7" max="7" width="16.88671875" style="11" customWidth="1"/>
-    <col min="8" max="8" width="15.77734375" style="11" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" style="11" customWidth="1"/>
-    <col min="10" max="16384" width="18.6640625" style="11"/>
+    <col min="1" max="1" width="10.453125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6328125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="16.1796875" style="7" customWidth="1"/>
+    <col min="4" max="4" width="18.36328125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="11.90625" style="7" customWidth="1"/>
+    <col min="6" max="6" width="15" style="7" customWidth="1"/>
+    <col min="7" max="7" width="16.90625" style="7" customWidth="1"/>
+    <col min="8" max="8" width="15.81640625" style="7" customWidth="1"/>
+    <col min="9" max="9" width="13.36328125" style="7" customWidth="1"/>
+    <col min="10" max="16384" width="18.6328125" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="6" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2921,45 +3351,45 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18.6640625" defaultRowHeight="16.2"/>
+  <sheetFormatPr defaultColWidth="18.6328125" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" style="11" customWidth="1"/>
-    <col min="2" max="2" width="6" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.21875" style="11" customWidth="1"/>
-    <col min="4" max="5" width="10.44140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15" style="11" customWidth="1"/>
-    <col min="7" max="7" width="16.88671875" style="11" customWidth="1"/>
-    <col min="8" max="8" width="15.77734375" style="11" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" style="11" customWidth="1"/>
-    <col min="10" max="16384" width="18.6640625" style="11"/>
+    <col min="1" max="1" width="13.90625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="6" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.1796875" style="7" customWidth="1"/>
+    <col min="4" max="5" width="10.453125" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" style="7" customWidth="1"/>
+    <col min="7" max="7" width="16.90625" style="7" customWidth="1"/>
+    <col min="8" max="8" width="15.81640625" style="7" customWidth="1"/>
+    <col min="9" max="9" width="13.36328125" style="7" customWidth="1"/>
+    <col min="10" max="16384" width="18.6328125" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="6" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2981,83 +3411,83 @@
       <selection activeCell="F9" sqref="F8:F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="8.33203125" style="17" customWidth="1"/>
-    <col min="2" max="2" width="15.77734375" style="18" customWidth="1"/>
-    <col min="3" max="3" width="15.5546875" style="18" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" style="18" customWidth="1"/>
-    <col min="5" max="5" width="16.109375" style="18" customWidth="1"/>
-    <col min="6" max="6" width="14.77734375" style="18" customWidth="1"/>
-    <col min="7" max="8" width="12.88671875" style="18" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" style="19" customWidth="1"/>
-    <col min="10" max="10" width="9" style="12"/>
-    <col min="11" max="16384" width="9" style="13"/>
+    <col min="1" max="1" width="8.36328125" style="13" customWidth="1"/>
+    <col min="2" max="2" width="15.81640625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="15.54296875" style="9" customWidth="1"/>
+    <col min="4" max="4" width="11.90625" style="9" customWidth="1"/>
+    <col min="5" max="5" width="16.08984375" style="9" customWidth="1"/>
+    <col min="6" max="6" width="14.81640625" style="9" customWidth="1"/>
+    <col min="7" max="8" width="12.90625" style="9" customWidth="1"/>
+    <col min="9" max="9" width="11.6328125" style="14" customWidth="1"/>
+    <col min="10" max="10" width="9" style="8"/>
+    <col min="11" max="16384" width="9" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="24.75" customHeight="1">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
     </row>
     <row r="2" spans="1:9" ht="24" customHeight="1">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="H2" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="I2" s="10" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="18.899999999999999" customHeight="1">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="16"/>
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="12"/>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="14"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="16"/>
+      <c r="A4" s="10"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3144,280 +3574,293 @@
   <sheetPr codeName="Sheet6">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P8"/>
+  <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="J14" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="9.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.44140625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="8.109375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="9" style="4"/>
-    <col min="5" max="5" width="8.33203125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="6.6640625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="8.109375" style="5" customWidth="1"/>
-    <col min="8" max="8" width="6.6640625" style="5" customWidth="1"/>
-    <col min="9" max="9" width="8.109375" style="5" customWidth="1"/>
-    <col min="10" max="10" width="6.6640625" style="5" customWidth="1"/>
-    <col min="11" max="11" width="8.109375" style="5" customWidth="1"/>
-    <col min="12" max="12" width="7.109375" style="6" customWidth="1"/>
-    <col min="13" max="13" width="8.109375" style="5" customWidth="1"/>
-    <col min="14" max="14" width="10" style="4" customWidth="1"/>
-    <col min="15" max="15" width="8.109375" style="7" customWidth="1"/>
-    <col min="16" max="16" width="7.88671875" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="9" style="1"/>
+    <col min="1" max="1" width="9.453125" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.453125" style="17" customWidth="1"/>
+    <col min="3" max="3" width="8.08984375" style="17" customWidth="1"/>
+    <col min="4" max="4" width="9" style="17"/>
+    <col min="5" max="5" width="8.36328125" style="17" customWidth="1"/>
+    <col min="6" max="6" width="6.6328125" style="34" customWidth="1"/>
+    <col min="7" max="7" width="8.08984375" style="34" customWidth="1"/>
+    <col min="8" max="8" width="6.6328125" style="34" customWidth="1"/>
+    <col min="9" max="9" width="8.08984375" style="34" customWidth="1"/>
+    <col min="10" max="10" width="6.6328125" style="34" customWidth="1"/>
+    <col min="11" max="11" width="8.08984375" style="34" customWidth="1"/>
+    <col min="12" max="12" width="7.08984375" style="35" customWidth="1"/>
+    <col min="13" max="13" width="8.08984375" style="34" customWidth="1"/>
+    <col min="14" max="14" width="10" style="17" customWidth="1"/>
+    <col min="15" max="15" width="8.08984375" style="36" customWidth="1"/>
+    <col min="16" max="16" width="7.90625" style="17" customWidth="1"/>
+    <col min="17" max="16384" width="9" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="18">
-      <c r="A1" s="37" t="s">
+    <row r="1" spans="1:15" ht="18.5">
+      <c r="A1" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
-    </row>
-    <row r="2" spans="1:16" ht="16.5" customHeight="1">
-      <c r="A2" s="39" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="39" t="s">
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+    </row>
+    <row r="2" spans="1:15" ht="16.5" customHeight="1">
+      <c r="A2" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="39" t="s">
+      <c r="D2" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="40" t="s">
+      <c r="E2" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="31" t="s">
+      <c r="F2" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31" t="s">
+      <c r="G2" s="20"/>
+      <c r="H2" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31" t="s">
+      <c r="I2" s="20"/>
+      <c r="J2" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31" t="s">
+      <c r="K2" s="20"/>
+      <c r="L2" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="M2" s="31"/>
-      <c r="N2" s="30" t="s">
+      <c r="M2" s="20"/>
+      <c r="N2" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="O2" s="38" t="s">
+      <c r="O2" s="22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:16" s="2" customFormat="1">
-      <c r="A3" s="39"/>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="20" t="s">
+    <row r="3" spans="1:15" s="24" customFormat="1">
+      <c r="A3" s="18"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="20" t="s">
+      <c r="H3" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="20" t="s">
+      <c r="I3" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="20" t="s">
+      <c r="J3" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="20" t="s">
+      <c r="K3" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="20" t="s">
+      <c r="L3" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="M3" s="20" t="s">
+      <c r="M3" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="N3" s="30"/>
-      <c r="O3" s="30"/>
-    </row>
-    <row r="4" spans="1:16">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="22"/>
-      <c r="L4" s="23"/>
-      <c r="M4" s="22"/>
-      <c r="N4" s="24"/>
-      <c r="O4" s="9"/>
-      <c r="P4" s="3"/>
-    </row>
-    <row r="5" spans="1:16">
-      <c r="A5" s="33" t="s">
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" s="25"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="28"/>
+      <c r="L4" s="29"/>
+      <c r="M4" s="28"/>
+      <c r="N4" s="30"/>
+      <c r="O4" s="26"/>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="33"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="25">
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="29">
         <f t="shared" ref="F5:K5" si="0">SUM(F4:F4)</f>
         <v>0</v>
       </c>
-      <c r="G5" s="25">
+      <c r="G5" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H5" s="25">
+      <c r="H5" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I5" s="26">
+      <c r="I5" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J5" s="25">
+      <c r="J5" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K5" s="25">
+      <c r="K5" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L5" s="25">
+      <c r="L5" s="29">
         <f>F5+H5+J5</f>
         <v>0</v>
       </c>
-      <c r="M5" s="26">
+      <c r="M5" s="28">
         <f>G5+I5+K5</f>
         <v>0</v>
       </c>
-      <c r="N5" s="27"/>
-      <c r="O5" s="28"/>
-    </row>
-    <row r="6" spans="1:16">
-      <c r="A6" s="33" t="s">
+      <c r="N5" s="25"/>
+      <c r="O5" s="31"/>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="33"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="35">
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="20">
         <f>SUBTOTAL(3,$C4:$C4)</f>
         <v>0</v>
       </c>
-      <c r="G6" s="35"/>
-      <c r="H6" s="36">
+      <c r="G6" s="20"/>
+      <c r="H6" s="32">
         <f>SUBTOTAL(3,$C4:$C4)</f>
         <v>0</v>
       </c>
-      <c r="I6" s="36"/>
-      <c r="J6" s="35">
+      <c r="I6" s="32"/>
+      <c r="J6" s="20">
         <f>SUBTOTAL(3,$C4:$C4)</f>
         <v>0</v>
       </c>
-      <c r="K6" s="35"/>
-      <c r="L6" s="35">
+      <c r="K6" s="20"/>
+      <c r="L6" s="20">
         <f>SUBTOTAL(3,$C4:$C4)</f>
         <v>0</v>
       </c>
-      <c r="M6" s="35"/>
-      <c r="N6" s="27"/>
-      <c r="O6" s="28"/>
-    </row>
-    <row r="7" spans="1:16">
-      <c r="A7" s="41" t="s">
+      <c r="M6" s="20"/>
+      <c r="N6" s="25"/>
+      <c r="O6" s="31"/>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="41"/>
-      <c r="C7" s="41"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="32">
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="20">
         <f>COUNTIF(F4:F4,"&lt;&gt;0")</f>
         <v>1</v>
       </c>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32">
+      <c r="G7" s="20"/>
+      <c r="H7" s="20">
         <f>COUNTIF(H4:H4,"&lt;&gt;0")</f>
         <v>1</v>
       </c>
-      <c r="I7" s="32"/>
-      <c r="J7" s="32">
+      <c r="I7" s="20"/>
+      <c r="J7" s="20">
         <f>COUNTIF(J4:J4,"&lt;&gt;0")</f>
         <v>1</v>
       </c>
-      <c r="K7" s="32"/>
-      <c r="L7" s="32">
+      <c r="K7" s="20"/>
+      <c r="L7" s="20">
         <f>COUNTIF(L4:L4,"&lt;&gt;0")</f>
         <v>1</v>
       </c>
-      <c r="M7" s="32"/>
-      <c r="N7" s="32"/>
-      <c r="O7" s="32"/>
-    </row>
-    <row r="8" spans="1:16">
-      <c r="A8" s="41" t="s">
+      <c r="M7" s="20"/>
+      <c r="N7" s="20"/>
+      <c r="O7" s="20"/>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="41"/>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="34" t="e">
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="33" t="e">
         <f>F7/F6</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34" t="e">
+      <c r="G8" s="33"/>
+      <c r="H8" s="33" t="e">
         <f>H7/H6</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I8" s="34"/>
-      <c r="J8" s="34" t="e">
+      <c r="I8" s="33"/>
+      <c r="J8" s="33" t="e">
         <f>J7/J6</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K8" s="34"/>
-      <c r="L8" s="34" t="e">
+      <c r="K8" s="33"/>
+      <c r="L8" s="33" t="e">
         <f>L7/L6</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M8" s="34"/>
-      <c r="N8" s="32"/>
-      <c r="O8" s="32"/>
+      <c r="M8" s="33"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="J7:K7"/>
     <mergeCell ref="A1:O1"/>
     <mergeCell ref="N8:O8"/>
     <mergeCell ref="J8:K8"/>
@@ -3434,20 +3877,6 @@
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="H8:I8"/>
     <mergeCell ref="A7:E7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="O4">
@@ -3484,280 +3913,500 @@
   <sheetPr codeName="Sheet7">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P8"/>
+  <dimension ref="A1:R17"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="R17" sqref="A1:R17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="9.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.44140625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="8.109375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="9" style="4"/>
-    <col min="5" max="5" width="8.33203125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="6.6640625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="8.109375" style="5" customWidth="1"/>
-    <col min="8" max="8" width="6.6640625" style="5" customWidth="1"/>
-    <col min="9" max="9" width="8.109375" style="5" customWidth="1"/>
-    <col min="10" max="10" width="6.6640625" style="5" customWidth="1"/>
-    <col min="11" max="11" width="8.109375" style="5" customWidth="1"/>
-    <col min="12" max="12" width="7.109375" style="6" customWidth="1"/>
-    <col min="13" max="13" width="8.109375" style="5" customWidth="1"/>
-    <col min="14" max="14" width="10" style="4" customWidth="1"/>
-    <col min="15" max="15" width="8.109375" style="7" customWidth="1"/>
-    <col min="16" max="16" width="7.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.453125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.08984375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9" style="1"/>
+    <col min="5" max="5" width="8.36328125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="6.6328125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="8.08984375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="6.6328125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="8.08984375" style="3" customWidth="1"/>
+    <col min="10" max="10" width="6.6328125" style="3" customWidth="1"/>
+    <col min="11" max="11" width="8.08984375" style="3" customWidth="1"/>
+    <col min="12" max="12" width="7.08984375" style="4" customWidth="1"/>
+    <col min="13" max="13" width="8.08984375" style="3" customWidth="1"/>
+    <col min="14" max="14" width="10" style="1" customWidth="1"/>
+    <col min="15" max="15" width="8.08984375" style="5" customWidth="1"/>
+    <col min="16" max="16" width="7.90625" style="1" customWidth="1"/>
     <col min="17" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="18">
-      <c r="A1" s="37" t="s">
+    <row r="1" spans="1:18" ht="18.5">
+      <c r="A1" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
-    </row>
-    <row r="2" spans="1:16" ht="16.5" customHeight="1">
-      <c r="A2" s="39" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="39" t="s">
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+    </row>
+    <row r="2" spans="1:18" ht="16.5" customHeight="1">
+      <c r="A2" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="39" t="s">
+      <c r="D2" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="40" t="s">
+      <c r="E2" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="31" t="s">
+      <c r="F2" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31" t="s">
+      <c r="G2" s="20"/>
+      <c r="H2" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31" t="s">
+      <c r="I2" s="20"/>
+      <c r="J2" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31" t="s">
+      <c r="K2" s="20"/>
+      <c r="L2" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="M2" s="31"/>
-      <c r="N2" s="30" t="s">
+      <c r="M2" s="20"/>
+      <c r="N2" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="O2" s="38" t="s">
+      <c r="O2" s="22" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" s="2" customFormat="1">
-      <c r="A3" s="39"/>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="20" t="s">
+      <c r="P2" s="17"/>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17"/>
+    </row>
+    <row r="3" spans="1:18" s="2" customFormat="1">
+      <c r="A3" s="18"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="20" t="s">
+      <c r="H3" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="20" t="s">
+      <c r="I3" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="20" t="s">
+      <c r="J3" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="20" t="s">
+      <c r="K3" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="20" t="s">
+      <c r="L3" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="M3" s="20" t="s">
+      <c r="M3" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="30"/>
-      <c r="O3" s="30"/>
-    </row>
-    <row r="4" spans="1:16">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="22"/>
-      <c r="L4" s="23"/>
-      <c r="M4" s="22"/>
-      <c r="N4" s="24"/>
-      <c r="O4" s="9"/>
-      <c r="P4" s="3"/>
-    </row>
-    <row r="5" spans="1:16">
-      <c r="A5" s="33" t="s">
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="24"/>
+      <c r="Q3" s="24"/>
+      <c r="R3" s="24"/>
+    </row>
+    <row r="4" spans="1:18">
+      <c r="A4" s="25"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="28"/>
+      <c r="L4" s="29"/>
+      <c r="M4" s="28"/>
+      <c r="N4" s="30"/>
+      <c r="O4" s="26"/>
+      <c r="P4" s="17"/>
+      <c r="Q4" s="17"/>
+      <c r="R4" s="17"/>
+    </row>
+    <row r="5" spans="1:18">
+      <c r="A5" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="33"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="25">
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="29">
         <f t="shared" ref="F5:K5" si="0">SUM(F4:F4)</f>
         <v>0</v>
       </c>
-      <c r="G5" s="25">
+      <c r="G5" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H5" s="25">
+      <c r="H5" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I5" s="26">
+      <c r="I5" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J5" s="25">
+      <c r="J5" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K5" s="25">
+      <c r="K5" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L5" s="25">
+      <c r="L5" s="29">
         <f>F5+H5+J5</f>
         <v>0</v>
       </c>
-      <c r="M5" s="26">
+      <c r="M5" s="28">
         <f>G5+I5+K5</f>
         <v>0</v>
       </c>
-      <c r="N5" s="27"/>
-      <c r="O5" s="28"/>
-    </row>
-    <row r="6" spans="1:16">
-      <c r="A6" s="33" t="s">
+      <c r="N5" s="25"/>
+      <c r="O5" s="31"/>
+      <c r="P5" s="17"/>
+      <c r="Q5" s="17"/>
+      <c r="R5" s="17"/>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="A6" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="33"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="35">
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="20">
         <f>SUBTOTAL(3,$C4:$C4)</f>
         <v>0</v>
       </c>
-      <c r="G6" s="35"/>
-      <c r="H6" s="36">
+      <c r="G6" s="20"/>
+      <c r="H6" s="32">
         <f>SUBTOTAL(3,$C4:$C4)</f>
         <v>0</v>
       </c>
-      <c r="I6" s="36"/>
-      <c r="J6" s="35">
+      <c r="I6" s="32"/>
+      <c r="J6" s="20">
         <f>SUBTOTAL(3,$C4:$C4)</f>
         <v>0</v>
       </c>
-      <c r="K6" s="35"/>
-      <c r="L6" s="35">
+      <c r="K6" s="20"/>
+      <c r="L6" s="20">
         <f>SUBTOTAL(3,$C4:$C4)</f>
         <v>0</v>
       </c>
-      <c r="M6" s="35"/>
-      <c r="N6" s="27"/>
-      <c r="O6" s="28"/>
-    </row>
-    <row r="7" spans="1:16">
-      <c r="A7" s="41" t="s">
+      <c r="M6" s="20"/>
+      <c r="N6" s="25"/>
+      <c r="O6" s="31"/>
+      <c r="P6" s="17"/>
+      <c r="Q6" s="17"/>
+      <c r="R6" s="17"/>
+    </row>
+    <row r="7" spans="1:18">
+      <c r="A7" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="41"/>
-      <c r="C7" s="41"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="32">
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="20">
         <f>COUNTIF(F4:F4,"&lt;&gt;0")</f>
         <v>1</v>
       </c>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32">
+      <c r="G7" s="20"/>
+      <c r="H7" s="20">
         <f>COUNTIF(H4:H4,"&lt;&gt;0")</f>
         <v>1</v>
       </c>
-      <c r="I7" s="32"/>
-      <c r="J7" s="32">
+      <c r="I7" s="20"/>
+      <c r="J7" s="20">
         <f>COUNTIF(J4:J4,"&lt;&gt;0")</f>
         <v>1</v>
       </c>
-      <c r="K7" s="32"/>
-      <c r="L7" s="32">
+      <c r="K7" s="20"/>
+      <c r="L7" s="20">
         <f>COUNTIF(L4:L4,"&lt;&gt;0")</f>
         <v>1</v>
       </c>
-      <c r="M7" s="32"/>
-      <c r="N7" s="32"/>
-      <c r="O7" s="32"/>
-    </row>
-    <row r="8" spans="1:16">
-      <c r="A8" s="41" t="s">
+      <c r="M7" s="20"/>
+      <c r="N7" s="20"/>
+      <c r="O7" s="20"/>
+      <c r="P7" s="17"/>
+      <c r="Q7" s="17"/>
+      <c r="R7" s="17"/>
+    </row>
+    <row r="8" spans="1:18">
+      <c r="A8" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="41"/>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="34" t="e">
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="33" t="e">
         <f>F7/F6</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34" t="e">
+      <c r="G8" s="33"/>
+      <c r="H8" s="33" t="e">
         <f>H7/H6</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I8" s="34"/>
-      <c r="J8" s="34" t="e">
+      <c r="I8" s="33"/>
+      <c r="J8" s="33" t="e">
         <f>J7/J6</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K8" s="34"/>
-      <c r="L8" s="34" t="e">
+      <c r="K8" s="33"/>
+      <c r="L8" s="33" t="e">
         <f>L7/L6</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M8" s="34"/>
-      <c r="N8" s="32"/>
-      <c r="O8" s="32"/>
+      <c r="M8" s="33"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="20"/>
+      <c r="P8" s="17"/>
+      <c r="Q8" s="17"/>
+      <c r="R8" s="17"/>
+    </row>
+    <row r="9" spans="1:18">
+      <c r="A9" s="17"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="34"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="34"/>
+      <c r="I9" s="34"/>
+      <c r="J9" s="34"/>
+      <c r="K9" s="34"/>
+      <c r="L9" s="35"/>
+      <c r="M9" s="34"/>
+      <c r="N9" s="17"/>
+      <c r="O9" s="36"/>
+      <c r="P9" s="17"/>
+      <c r="Q9" s="17"/>
+      <c r="R9" s="17"/>
+    </row>
+    <row r="10" spans="1:18">
+      <c r="A10" s="17"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="34"/>
+      <c r="I10" s="34"/>
+      <c r="J10" s="34"/>
+      <c r="K10" s="34"/>
+      <c r="L10" s="35"/>
+      <c r="M10" s="34"/>
+      <c r="N10" s="17"/>
+      <c r="O10" s="36"/>
+      <c r="P10" s="17"/>
+      <c r="Q10" s="17"/>
+      <c r="R10" s="17"/>
+    </row>
+    <row r="11" spans="1:18">
+      <c r="A11" s="17"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="34"/>
+      <c r="J11" s="34"/>
+      <c r="K11" s="34"/>
+      <c r="L11" s="35"/>
+      <c r="M11" s="34"/>
+      <c r="N11" s="17"/>
+      <c r="O11" s="36"/>
+      <c r="P11" s="17"/>
+      <c r="Q11" s="17"/>
+      <c r="R11" s="17"/>
+    </row>
+    <row r="12" spans="1:18">
+      <c r="A12" s="17"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
+      <c r="J12" s="34"/>
+      <c r="K12" s="34"/>
+      <c r="L12" s="35"/>
+      <c r="M12" s="34"/>
+      <c r="N12" s="17"/>
+      <c r="O12" s="36"/>
+      <c r="P12" s="17"/>
+      <c r="Q12" s="17"/>
+      <c r="R12" s="17"/>
+    </row>
+    <row r="13" spans="1:18">
+      <c r="A13" s="17"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="34"/>
+      <c r="I13" s="34"/>
+      <c r="J13" s="34"/>
+      <c r="K13" s="34"/>
+      <c r="L13" s="35"/>
+      <c r="M13" s="34"/>
+      <c r="N13" s="17"/>
+      <c r="O13" s="36"/>
+      <c r="P13" s="17"/>
+      <c r="Q13" s="17"/>
+      <c r="R13" s="17"/>
+    </row>
+    <row r="14" spans="1:18">
+      <c r="A14" s="17"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="34"/>
+      <c r="K14" s="34"/>
+      <c r="L14" s="35"/>
+      <c r="M14" s="34"/>
+      <c r="N14" s="17"/>
+      <c r="O14" s="36"/>
+      <c r="P14" s="17"/>
+      <c r="Q14" s="17"/>
+      <c r="R14" s="17"/>
+    </row>
+    <row r="15" spans="1:18">
+      <c r="A15" s="17"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="34"/>
+      <c r="I15" s="34"/>
+      <c r="J15" s="34"/>
+      <c r="K15" s="34"/>
+      <c r="L15" s="35"/>
+      <c r="M15" s="34"/>
+      <c r="N15" s="17"/>
+      <c r="O15" s="36"/>
+      <c r="P15" s="17"/>
+      <c r="Q15" s="17"/>
+      <c r="R15" s="17"/>
+    </row>
+    <row r="16" spans="1:18">
+      <c r="A16" s="17"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="34"/>
+      <c r="J16" s="34"/>
+      <c r="K16" s="34"/>
+      <c r="L16" s="35"/>
+      <c r="M16" s="34"/>
+      <c r="N16" s="17"/>
+      <c r="O16" s="36"/>
+      <c r="P16" s="17"/>
+      <c r="Q16" s="17"/>
+      <c r="R16" s="17"/>
+    </row>
+    <row r="17" spans="1:18">
+      <c r="A17" s="17"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="34"/>
+      <c r="H17" s="34"/>
+      <c r="I17" s="34"/>
+      <c r="J17" s="34"/>
+      <c r="K17" s="34"/>
+      <c r="L17" s="35"/>
+      <c r="M17" s="34"/>
+      <c r="N17" s="17"/>
+      <c r="O17" s="36"/>
+      <c r="P17" s="17"/>
+      <c r="Q17" s="17"/>
+      <c r="R17" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="O2:O3"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:K6"/>
     <mergeCell ref="L6:M6"/>
     <mergeCell ref="N8:O8"/>
     <mergeCell ref="A7:E7"/>
@@ -3771,23 +4420,6 @@
     <mergeCell ref="H8:I8"/>
     <mergeCell ref="J8:K8"/>
     <mergeCell ref="L8:M8"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="A1:O1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="O2:O3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="O4">

</xml_diff>

<commit_message>
Auto-committed on 2023/06/06 週二 11:25:06.80
</commit_message>
<xml_diff>
--- a/Program/Other/LP005_底稿_協辦考核核算.xlsx
+++ b/Program/Other/LP005_底稿_協辦考核核算.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SVN\iTX\Other\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LINDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52F485CE-8C0B-41B7-9B93-5F2B325BC3EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ED53644-2E2C-4D20-9DC9-261CC87C7A62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" tabRatio="791" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="791" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1月件數" sheetId="70" r:id="rId1"/>
@@ -837,7 +837,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -883,95 +883,56 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="10" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1765,22 +1726,20 @@
   <sheetPr codeName="工作表1"/>
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18.6328125" defaultRowHeight="17"/>
+  <sheetFormatPr defaultColWidth="18.6640625" defaultRowHeight="16.2"/>
   <cols>
-    <col min="1" max="1" width="10.453125" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.6328125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="16.1796875" style="7" customWidth="1"/>
-    <col min="4" max="4" width="18.36328125" style="7" customWidth="1"/>
-    <col min="5" max="5" width="11.90625" style="7" customWidth="1"/>
+    <col min="1" max="1" width="10.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="16.21875" style="7" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" style="7" customWidth="1"/>
     <col min="6" max="6" width="15" style="7" customWidth="1"/>
-    <col min="7" max="7" width="16.90625" style="7" customWidth="1"/>
-    <col min="8" max="8" width="15.81640625" style="7" customWidth="1"/>
-    <col min="9" max="9" width="13.36328125" style="7" customWidth="1"/>
-    <col min="10" max="16384" width="18.6328125" style="7"/>
+    <col min="7" max="7" width="16.88671875" style="7" customWidth="1"/>
+    <col min="8" max="8" width="15.77734375" style="7" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" style="7" customWidth="1"/>
+    <col min="10" max="16384" width="18.6640625" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -1824,449 +1783,279 @@
   <sheetPr codeName="Sheet8">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O17"/>
+  <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N17" sqref="A1:O17"/>
+      <selection sqref="A1:O1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.453125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.08984375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="9" style="1"/>
-    <col min="5" max="5" width="8.36328125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="6.6328125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="8.08984375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="6.6328125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="8.08984375" style="3" customWidth="1"/>
-    <col min="10" max="10" width="6.6328125" style="3" customWidth="1"/>
-    <col min="11" max="11" width="8.08984375" style="3" customWidth="1"/>
-    <col min="12" max="12" width="7.08984375" style="4" customWidth="1"/>
-    <col min="13" max="13" width="8.08984375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="6.6640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="8.109375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="6.6640625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="8.109375" style="3" customWidth="1"/>
+    <col min="10" max="10" width="6.6640625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="8.109375" style="3" customWidth="1"/>
+    <col min="12" max="12" width="7.109375" style="4" customWidth="1"/>
+    <col min="13" max="13" width="8.109375" style="3" customWidth="1"/>
     <col min="14" max="14" width="10" style="1" customWidth="1"/>
-    <col min="15" max="15" width="8.08984375" style="5" customWidth="1"/>
-    <col min="16" max="16" width="7.90625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="8.109375" style="5" customWidth="1"/>
+    <col min="16" max="16" width="7.88671875" style="1" customWidth="1"/>
     <col min="17" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="18.5">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:15" ht="18">
+      <c r="A1" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
     </row>
     <row r="2" spans="1:15" ht="16.5" customHeight="1">
-      <c r="A2" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="18" t="s">
+      <c r="A2" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20" t="s">
+      <c r="G2" s="25"/>
+      <c r="H2" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20" t="s">
+      <c r="I2" s="25"/>
+      <c r="J2" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20" t="s">
+      <c r="K2" s="25"/>
+      <c r="L2" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="M2" s="20"/>
-      <c r="N2" s="21" t="s">
+      <c r="M2" s="25"/>
+      <c r="N2" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="O2" s="22" t="s">
+      <c r="O2" s="29" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:15" s="2" customFormat="1">
-      <c r="A3" s="18"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="23" t="s">
+      <c r="A3" s="30"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="G3" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="23" t="s">
+      <c r="H3" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="23" t="s">
+      <c r="I3" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="23" t="s">
+      <c r="J3" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="23" t="s">
+      <c r="K3" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="23" t="s">
+      <c r="L3" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="M3" s="23" t="s">
+      <c r="M3" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="21"/>
-      <c r="O3" s="21"/>
+      <c r="N3" s="24"/>
+      <c r="O3" s="24"/>
     </row>
     <row r="4" spans="1:15">
-      <c r="A4" s="25"/>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="28"/>
-      <c r="J4" s="29"/>
-      <c r="K4" s="28"/>
-      <c r="L4" s="29"/>
-      <c r="M4" s="28"/>
-      <c r="N4" s="30"/>
-      <c r="O4" s="26"/>
+      <c r="A4" s="17"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="18"/>
     </row>
     <row r="5" spans="1:15">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="29">
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="21">
         <f t="shared" ref="F5:K5" si="0">SUM(F4:F4)</f>
         <v>0</v>
       </c>
-      <c r="G5" s="29">
+      <c r="G5" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H5" s="29">
+      <c r="H5" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I5" s="28">
+      <c r="I5" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J5" s="29">
+      <c r="J5" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K5" s="29">
+      <c r="K5" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L5" s="29">
+      <c r="L5" s="21">
         <f>F5+H5+J5</f>
         <v>0</v>
       </c>
-      <c r="M5" s="28">
+      <c r="M5" s="20">
         <f>G5+I5+K5</f>
         <v>0</v>
       </c>
-      <c r="N5" s="25"/>
-      <c r="O5" s="31"/>
+      <c r="N5" s="17"/>
+      <c r="O5" s="22"/>
     </row>
     <row r="6" spans="1:15">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="20">
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="25">
         <f>SUBTOTAL(3,$C4:$C4)</f>
         <v>0</v>
       </c>
-      <c r="G6" s="20"/>
-      <c r="H6" s="32">
+      <c r="G6" s="25"/>
+      <c r="H6" s="27">
         <f>SUBTOTAL(3,$C4:$C4)</f>
         <v>0</v>
       </c>
-      <c r="I6" s="32"/>
-      <c r="J6" s="20">
+      <c r="I6" s="27"/>
+      <c r="J6" s="25">
         <f>SUBTOTAL(3,$C4:$C4)</f>
         <v>0</v>
       </c>
-      <c r="K6" s="20"/>
-      <c r="L6" s="20">
+      <c r="K6" s="25"/>
+      <c r="L6" s="25">
         <f>SUBTOTAL(3,$C4:$C4)</f>
         <v>0</v>
       </c>
-      <c r="M6" s="20"/>
-      <c r="N6" s="25"/>
-      <c r="O6" s="31"/>
+      <c r="M6" s="25"/>
+      <c r="N6" s="17"/>
+      <c r="O6" s="22"/>
     </row>
     <row r="7" spans="1:15">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="20">
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="25">
         <f>COUNTIF(F4:F4,"&lt;&gt;0")</f>
         <v>1</v>
       </c>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20">
+      <c r="G7" s="25"/>
+      <c r="H7" s="25">
         <f>COUNTIF(H4:H4,"&lt;&gt;0")</f>
         <v>1</v>
       </c>
-      <c r="I7" s="20"/>
-      <c r="J7" s="20">
+      <c r="I7" s="25"/>
+      <c r="J7" s="25">
         <f>COUNTIF(J4:J4,"&lt;&gt;0")</f>
         <v>1</v>
       </c>
-      <c r="K7" s="20"/>
-      <c r="L7" s="20">
+      <c r="K7" s="25"/>
+      <c r="L7" s="25">
         <f>COUNTIF(L4:L4,"&lt;&gt;0")</f>
         <v>1</v>
       </c>
-      <c r="M7" s="20"/>
-      <c r="N7" s="20"/>
-      <c r="O7" s="20"/>
+      <c r="M7" s="25"/>
+      <c r="N7" s="25"/>
+      <c r="O7" s="25"/>
     </row>
     <row r="8" spans="1:15">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="33" t="e">
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="26" t="e">
         <f>F7/F6</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G8" s="33"/>
-      <c r="H8" s="33" t="e">
+      <c r="G8" s="26"/>
+      <c r="H8" s="26" t="e">
         <f>H7/H6</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I8" s="33"/>
-      <c r="J8" s="33" t="e">
+      <c r="I8" s="26"/>
+      <c r="J8" s="26" t="e">
         <f>J7/J6</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K8" s="33"/>
-      <c r="L8" s="33" t="e">
+      <c r="K8" s="26"/>
+      <c r="L8" s="26" t="e">
         <f>L7/L6</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M8" s="33"/>
-      <c r="N8" s="20"/>
-      <c r="O8" s="20"/>
-    </row>
-    <row r="9" spans="1:15">
-      <c r="A9" s="17"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="34"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="34"/>
-      <c r="J9" s="34"/>
-      <c r="K9" s="34"/>
-      <c r="L9" s="35"/>
-      <c r="M9" s="34"/>
-      <c r="N9" s="17"/>
-      <c r="O9" s="36"/>
-    </row>
-    <row r="10" spans="1:15">
-      <c r="A10" s="17"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="34"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="34"/>
-      <c r="J10" s="34"/>
-      <c r="K10" s="34"/>
-      <c r="L10" s="35"/>
-      <c r="M10" s="34"/>
-      <c r="N10" s="17"/>
-      <c r="O10" s="36"/>
-    </row>
-    <row r="11" spans="1:15">
-      <c r="A11" s="17"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="34"/>
-      <c r="J11" s="34"/>
-      <c r="K11" s="34"/>
-      <c r="L11" s="35"/>
-      <c r="M11" s="34"/>
-      <c r="N11" s="17"/>
-      <c r="O11" s="36"/>
-    </row>
-    <row r="12" spans="1:15">
-      <c r="A12" s="17"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="34"/>
-      <c r="J12" s="34"/>
-      <c r="K12" s="34"/>
-      <c r="L12" s="35"/>
-      <c r="M12" s="34"/>
-      <c r="N12" s="17"/>
-      <c r="O12" s="36"/>
-    </row>
-    <row r="13" spans="1:15">
-      <c r="A13" s="17"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="34"/>
-      <c r="G13" s="34"/>
-      <c r="H13" s="34"/>
-      <c r="I13" s="34"/>
-      <c r="J13" s="34"/>
-      <c r="K13" s="34"/>
-      <c r="L13" s="35"/>
-      <c r="M13" s="34"/>
-      <c r="N13" s="17"/>
-      <c r="O13" s="36"/>
-    </row>
-    <row r="14" spans="1:15">
-      <c r="A14" s="17"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="34"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="34"/>
-      <c r="J14" s="34"/>
-      <c r="K14" s="34"/>
-      <c r="L14" s="35"/>
-      <c r="M14" s="34"/>
-      <c r="N14" s="17"/>
-      <c r="O14" s="36"/>
-    </row>
-    <row r="15" spans="1:15">
-      <c r="A15" s="17"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="34"/>
-      <c r="J15" s="34"/>
-      <c r="K15" s="34"/>
-      <c r="L15" s="35"/>
-      <c r="M15" s="34"/>
-      <c r="N15" s="17"/>
-      <c r="O15" s="36"/>
-    </row>
-    <row r="16" spans="1:15">
-      <c r="A16" s="17"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="34"/>
-      <c r="J16" s="34"/>
-      <c r="K16" s="34"/>
-      <c r="L16" s="35"/>
-      <c r="M16" s="34"/>
-      <c r="N16" s="17"/>
-      <c r="O16" s="36"/>
-    </row>
-    <row r="17" spans="1:15">
-      <c r="A17" s="17"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="34"/>
-      <c r="G17" s="34"/>
-      <c r="H17" s="34"/>
-      <c r="I17" s="34"/>
-      <c r="J17" s="34"/>
-      <c r="K17" s="34"/>
-      <c r="L17" s="35"/>
-      <c r="M17" s="34"/>
-      <c r="N17" s="17"/>
-      <c r="O17" s="36"/>
+      <c r="M8" s="26"/>
+      <c r="N8" s="25"/>
+      <c r="O8" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="A1:O1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="O2:O3"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
     <mergeCell ref="L6:M6"/>
     <mergeCell ref="N8:O8"/>
     <mergeCell ref="A7:E7"/>
@@ -2280,6 +2069,23 @@
     <mergeCell ref="H8:I8"/>
     <mergeCell ref="J8:K8"/>
     <mergeCell ref="L8:M8"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="O2:O3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="O4">
@@ -2316,466 +2122,279 @@
   <sheetPr codeName="Sheet9">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P17"/>
+  <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P17" sqref="A1:P17"/>
+      <selection sqref="A1:O1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.453125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.08984375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="9" style="1"/>
-    <col min="5" max="5" width="8.36328125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="6.6328125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="8.08984375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="6.6328125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="8.08984375" style="3" customWidth="1"/>
-    <col min="10" max="10" width="6.6328125" style="3" customWidth="1"/>
-    <col min="11" max="11" width="8.08984375" style="3" customWidth="1"/>
-    <col min="12" max="12" width="7.08984375" style="4" customWidth="1"/>
-    <col min="13" max="13" width="8.08984375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="6.6640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="8.109375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="6.6640625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="8.109375" style="3" customWidth="1"/>
+    <col min="10" max="10" width="6.6640625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="8.109375" style="3" customWidth="1"/>
+    <col min="12" max="12" width="7.109375" style="4" customWidth="1"/>
+    <col min="13" max="13" width="8.109375" style="3" customWidth="1"/>
     <col min="14" max="14" width="10" style="1" customWidth="1"/>
-    <col min="15" max="15" width="8.08984375" style="5" customWidth="1"/>
-    <col min="16" max="16" width="7.90625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="8.109375" style="5" customWidth="1"/>
+    <col min="16" max="16" width="7.88671875" style="1" customWidth="1"/>
     <col min="17" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="18.5">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:15" ht="18">
+      <c r="A1" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
-      <c r="P1" s="17"/>
-    </row>
-    <row r="2" spans="1:16" ht="16.5" customHeight="1">
-      <c r="A2" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="18" t="s">
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+    </row>
+    <row r="2" spans="1:15" ht="16.5" customHeight="1">
+      <c r="A2" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20" t="s">
+      <c r="G2" s="25"/>
+      <c r="H2" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20" t="s">
+      <c r="I2" s="25"/>
+      <c r="J2" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20" t="s">
+      <c r="K2" s="25"/>
+      <c r="L2" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="M2" s="20"/>
-      <c r="N2" s="21" t="s">
+      <c r="M2" s="25"/>
+      <c r="N2" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="O2" s="22" t="s">
+      <c r="O2" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="P2" s="17"/>
-    </row>
-    <row r="3" spans="1:16" s="2" customFormat="1">
-      <c r="A3" s="18"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="23" t="s">
+    </row>
+    <row r="3" spans="1:15" s="2" customFormat="1">
+      <c r="A3" s="30"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="G3" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="23" t="s">
+      <c r="H3" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="23" t="s">
+      <c r="I3" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="23" t="s">
+      <c r="J3" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="23" t="s">
+      <c r="K3" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="23" t="s">
+      <c r="L3" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="M3" s="23" t="s">
+      <c r="M3" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="21"/>
-      <c r="O3" s="21"/>
-      <c r="P3" s="24"/>
-    </row>
-    <row r="4" spans="1:16">
-      <c r="A4" s="25"/>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="28"/>
-      <c r="J4" s="29"/>
-      <c r="K4" s="28"/>
-      <c r="L4" s="29"/>
-      <c r="M4" s="28"/>
-      <c r="N4" s="30"/>
-      <c r="O4" s="26"/>
-      <c r="P4" s="17"/>
-    </row>
-    <row r="5" spans="1:16">
-      <c r="A5" s="21" t="s">
+      <c r="N3" s="24"/>
+      <c r="O3" s="24"/>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" s="17"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="18"/>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="29">
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="21">
         <f t="shared" ref="F5:K5" si="0">SUM(F4:F4)</f>
         <v>0</v>
       </c>
-      <c r="G5" s="29">
+      <c r="G5" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H5" s="29">
+      <c r="H5" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I5" s="28">
+      <c r="I5" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J5" s="29">
+      <c r="J5" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K5" s="29">
+      <c r="K5" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L5" s="29">
+      <c r="L5" s="21">
         <f>F5+H5+J5</f>
         <v>0</v>
       </c>
-      <c r="M5" s="28">
+      <c r="M5" s="20">
         <f>G5+I5+K5</f>
         <v>0</v>
       </c>
-      <c r="N5" s="25"/>
-      <c r="O5" s="31"/>
-      <c r="P5" s="17"/>
-    </row>
-    <row r="6" spans="1:16">
-      <c r="A6" s="21" t="s">
+      <c r="N5" s="17"/>
+      <c r="O5" s="22"/>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="20">
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="25">
         <f>SUBTOTAL(3,$C4:$C4)</f>
         <v>0</v>
       </c>
-      <c r="G6" s="20"/>
-      <c r="H6" s="32">
+      <c r="G6" s="25"/>
+      <c r="H6" s="27">
         <f>SUBTOTAL(3,$C4:$C4)</f>
         <v>0</v>
       </c>
-      <c r="I6" s="32"/>
-      <c r="J6" s="20">
+      <c r="I6" s="27"/>
+      <c r="J6" s="25">
         <f>SUBTOTAL(3,$C4:$C4)</f>
         <v>0</v>
       </c>
-      <c r="K6" s="20"/>
-      <c r="L6" s="20">
+      <c r="K6" s="25"/>
+      <c r="L6" s="25">
         <f>SUBTOTAL(3,$C4:$C4)</f>
         <v>0</v>
       </c>
-      <c r="M6" s="20"/>
-      <c r="N6" s="25"/>
-      <c r="O6" s="31"/>
-      <c r="P6" s="17"/>
-    </row>
-    <row r="7" spans="1:16">
-      <c r="A7" s="21" t="s">
+      <c r="M6" s="25"/>
+      <c r="N6" s="17"/>
+      <c r="O6" s="22"/>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="20">
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="25">
         <f>COUNTIF(F4:F4,"&lt;&gt;0")</f>
         <v>1</v>
       </c>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20">
+      <c r="G7" s="25"/>
+      <c r="H7" s="25">
         <f>COUNTIF(H4:H4,"&lt;&gt;0")</f>
         <v>1</v>
       </c>
-      <c r="I7" s="20"/>
-      <c r="J7" s="20">
+      <c r="I7" s="25"/>
+      <c r="J7" s="25">
         <f>COUNTIF(J4:J4,"&lt;&gt;0")</f>
         <v>1</v>
       </c>
-      <c r="K7" s="20"/>
-      <c r="L7" s="20">
+      <c r="K7" s="25"/>
+      <c r="L7" s="25">
         <f>COUNTIF(L4:L4,"&lt;&gt;0")</f>
         <v>1</v>
       </c>
-      <c r="M7" s="20"/>
-      <c r="N7" s="20"/>
-      <c r="O7" s="20"/>
-      <c r="P7" s="17"/>
-    </row>
-    <row r="8" spans="1:16">
-      <c r="A8" s="21" t="s">
+      <c r="M7" s="25"/>
+      <c r="N7" s="25"/>
+      <c r="O7" s="25"/>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="33" t="e">
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="26" t="e">
         <f>F7/F6</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G8" s="33"/>
-      <c r="H8" s="33" t="e">
+      <c r="G8" s="26"/>
+      <c r="H8" s="26" t="e">
         <f>H7/H6</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I8" s="33"/>
-      <c r="J8" s="33" t="e">
+      <c r="I8" s="26"/>
+      <c r="J8" s="26" t="e">
         <f>J7/J6</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K8" s="33"/>
-      <c r="L8" s="33" t="e">
+      <c r="K8" s="26"/>
+      <c r="L8" s="26" t="e">
         <f>L7/L6</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M8" s="33"/>
-      <c r="N8" s="20"/>
-      <c r="O8" s="20"/>
-      <c r="P8" s="17"/>
-    </row>
-    <row r="9" spans="1:16">
-      <c r="A9" s="17"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="34"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="34"/>
-      <c r="J9" s="34"/>
-      <c r="K9" s="34"/>
-      <c r="L9" s="35"/>
-      <c r="M9" s="34"/>
-      <c r="N9" s="17"/>
-      <c r="O9" s="36"/>
-      <c r="P9" s="17"/>
-    </row>
-    <row r="10" spans="1:16">
-      <c r="A10" s="17"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="34"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="34"/>
-      <c r="J10" s="34"/>
-      <c r="K10" s="34"/>
-      <c r="L10" s="35"/>
-      <c r="M10" s="34"/>
-      <c r="N10" s="17"/>
-      <c r="O10" s="36"/>
-      <c r="P10" s="17"/>
-    </row>
-    <row r="11" spans="1:16">
-      <c r="A11" s="17"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="34"/>
-      <c r="J11" s="34"/>
-      <c r="K11" s="34"/>
-      <c r="L11" s="35"/>
-      <c r="M11" s="34"/>
-      <c r="N11" s="17"/>
-      <c r="O11" s="36"/>
-      <c r="P11" s="17"/>
-    </row>
-    <row r="12" spans="1:16">
-      <c r="A12" s="17"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="34"/>
-      <c r="J12" s="34"/>
-      <c r="K12" s="34"/>
-      <c r="L12" s="35"/>
-      <c r="M12" s="34"/>
-      <c r="N12" s="17"/>
-      <c r="O12" s="36"/>
-      <c r="P12" s="17"/>
-    </row>
-    <row r="13" spans="1:16">
-      <c r="A13" s="17"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="34"/>
-      <c r="G13" s="34"/>
-      <c r="H13" s="34"/>
-      <c r="I13" s="34"/>
-      <c r="J13" s="34"/>
-      <c r="K13" s="34"/>
-      <c r="L13" s="35"/>
-      <c r="M13" s="34"/>
-      <c r="N13" s="17"/>
-      <c r="O13" s="36"/>
-      <c r="P13" s="17"/>
-    </row>
-    <row r="14" spans="1:16">
-      <c r="A14" s="17"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="34"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="34"/>
-      <c r="J14" s="34"/>
-      <c r="K14" s="34"/>
-      <c r="L14" s="35"/>
-      <c r="M14" s="34"/>
-      <c r="N14" s="17"/>
-      <c r="O14" s="36"/>
-      <c r="P14" s="17"/>
-    </row>
-    <row r="15" spans="1:16">
-      <c r="A15" s="17"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="34"/>
-      <c r="J15" s="34"/>
-      <c r="K15" s="34"/>
-      <c r="L15" s="35"/>
-      <c r="M15" s="34"/>
-      <c r="N15" s="17"/>
-      <c r="O15" s="36"/>
-      <c r="P15" s="17"/>
-    </row>
-    <row r="16" spans="1:16">
-      <c r="A16" s="17"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="34"/>
-      <c r="J16" s="34"/>
-      <c r="K16" s="34"/>
-      <c r="L16" s="35"/>
-      <c r="M16" s="34"/>
-      <c r="N16" s="17"/>
-      <c r="O16" s="36"/>
-      <c r="P16" s="17"/>
-    </row>
-    <row r="17" spans="1:16">
-      <c r="A17" s="17"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="34"/>
-      <c r="G17" s="34"/>
-      <c r="H17" s="34"/>
-      <c r="I17" s="34"/>
-      <c r="J17" s="34"/>
-      <c r="K17" s="34"/>
-      <c r="L17" s="35"/>
-      <c r="M17" s="34"/>
-      <c r="N17" s="17"/>
-      <c r="O17" s="36"/>
-      <c r="P17" s="17"/>
+      <c r="M8" s="26"/>
+      <c r="N8" s="25"/>
+      <c r="O8" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="A1:O1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="O2:O3"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
     <mergeCell ref="L6:M6"/>
     <mergeCell ref="N8:O8"/>
     <mergeCell ref="A7:E7"/>
@@ -2789,6 +2408,23 @@
     <mergeCell ref="H8:I8"/>
     <mergeCell ref="J8:K8"/>
     <mergeCell ref="L8:M8"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="O2:O3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="O4">
@@ -2825,213 +2461,89 @@
   <sheetPr codeName="工作表5">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J14" sqref="A1:J14"/>
+      <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.2"/>
   <cols>
-    <col min="1" max="1" width="8.36328125" style="13" customWidth="1"/>
-    <col min="2" max="2" width="15.81640625" style="9" customWidth="1"/>
-    <col min="3" max="3" width="15.54296875" style="9" customWidth="1"/>
-    <col min="4" max="4" width="11.90625" style="9" customWidth="1"/>
-    <col min="5" max="5" width="16.08984375" style="9" customWidth="1"/>
-    <col min="6" max="6" width="14.81640625" style="9" customWidth="1"/>
-    <col min="7" max="8" width="12.90625" style="9" customWidth="1"/>
-    <col min="9" max="9" width="11.6328125" style="14" customWidth="1"/>
+    <col min="1" max="1" width="8.33203125" style="13" customWidth="1"/>
+    <col min="2" max="2" width="15.77734375" style="9" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" style="9" customWidth="1"/>
+    <col min="4" max="4" width="11.88671875" style="9" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" style="9" customWidth="1"/>
+    <col min="6" max="6" width="14.77734375" style="9" customWidth="1"/>
+    <col min="7" max="8" width="12.88671875" style="9" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" style="14" customWidth="1"/>
     <col min="10" max="10" width="9" style="8"/>
     <col min="11" max="16384" width="9" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="24.75" customHeight="1">
-      <c r="A1" s="37" t="s">
+    <row r="1" spans="1:9" ht="24.75" customHeight="1">
+      <c r="A1" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="38"/>
-    </row>
-    <row r="2" spans="1:10" ht="24" customHeight="1">
-      <c r="A2" s="39" t="s">
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+    </row>
+    <row r="2" spans="1:9" ht="24" customHeight="1">
+      <c r="A2" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="39" t="s">
+      <c r="D2" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E2" s="39" t="s">
+      <c r="E2" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F2" s="39" t="s">
+      <c r="F2" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="40" t="s">
+      <c r="G2" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="H2" s="40" t="s">
+      <c r="H2" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="I2" s="39" t="s">
+      <c r="I2" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J2" s="38"/>
-    </row>
-    <row r="3" spans="1:10" ht="18.899999999999999" customHeight="1">
-      <c r="A3" s="39"/>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="38"/>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="39"/>
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="41"/>
-      <c r="J4" s="38"/>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="42"/>
-      <c r="B5" s="43"/>
-      <c r="C5" s="43"/>
-      <c r="D5" s="43"/>
-      <c r="E5" s="43"/>
-      <c r="F5" s="43"/>
-      <c r="G5" s="43"/>
-      <c r="H5" s="43"/>
-      <c r="I5" s="44"/>
-      <c r="J5" s="38"/>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="42"/>
-      <c r="B6" s="43"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="43"/>
-      <c r="I6" s="44"/>
-      <c r="J6" s="38"/>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="42"/>
-      <c r="B7" s="43"/>
-      <c r="C7" s="43"/>
-      <c r="D7" s="43"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="43"/>
-      <c r="G7" s="43"/>
-      <c r="H7" s="43"/>
-      <c r="I7" s="44"/>
-      <c r="J7" s="38"/>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="42"/>
-      <c r="B8" s="43"/>
-      <c r="C8" s="43"/>
-      <c r="D8" s="43"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="43"/>
-      <c r="H8" s="43"/>
-      <c r="I8" s="44"/>
-      <c r="J8" s="38"/>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="42"/>
-      <c r="B9" s="43"/>
-      <c r="C9" s="43"/>
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="44"/>
-      <c r="J9" s="38"/>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="42"/>
-      <c r="B10" s="43"/>
-      <c r="C10" s="43"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="43"/>
-      <c r="H10" s="43"/>
-      <c r="I10" s="44"/>
-      <c r="J10" s="38"/>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11" s="42"/>
-      <c r="B11" s="43"/>
-      <c r="C11" s="43"/>
-      <c r="D11" s="43"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="43"/>
-      <c r="H11" s="43"/>
-      <c r="I11" s="44"/>
-      <c r="J11" s="38"/>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12" s="42"/>
-      <c r="B12" s="43"/>
-      <c r="C12" s="43"/>
-      <c r="D12" s="43"/>
-      <c r="E12" s="43"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="43"/>
-      <c r="H12" s="43"/>
-      <c r="I12" s="44"/>
-      <c r="J12" s="38"/>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="A13" s="42"/>
-      <c r="B13" s="43"/>
-      <c r="C13" s="43"/>
-      <c r="D13" s="43"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="43"/>
-      <c r="H13" s="43"/>
-      <c r="I13" s="44"/>
-      <c r="J13" s="38"/>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" s="42"/>
-      <c r="B14" s="43"/>
-      <c r="C14" s="43"/>
-      <c r="D14" s="43"/>
-      <c r="E14" s="43"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="43"/>
-      <c r="H14" s="43"/>
-      <c r="I14" s="44"/>
-      <c r="J14" s="38"/>
+    </row>
+    <row r="3" spans="1:9" ht="18.899999999999999" customHeight="1">
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="12"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="10"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3117,21 +2629,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F5A011B-B6C8-45CD-9219-0AEAA3A08C8A}">
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18.6328125" defaultRowHeight="17"/>
+  <sheetFormatPr defaultColWidth="18.6640625" defaultRowHeight="16.2"/>
   <cols>
-    <col min="1" max="1" width="13.90625" style="7" customWidth="1"/>
+    <col min="1" max="1" width="13.88671875" style="7" customWidth="1"/>
     <col min="2" max="2" width="6" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.1796875" style="7" customWidth="1"/>
-    <col min="4" max="5" width="10.453125" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.21875" style="7" customWidth="1"/>
+    <col min="4" max="5" width="10.44140625" style="7" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" style="7" customWidth="1"/>
-    <col min="7" max="7" width="16.90625" style="7" customWidth="1"/>
-    <col min="8" max="8" width="15.81640625" style="7" customWidth="1"/>
-    <col min="9" max="9" width="13.36328125" style="7" customWidth="1"/>
-    <col min="10" max="16384" width="18.6328125" style="7"/>
+    <col min="7" max="7" width="16.88671875" style="7" customWidth="1"/>
+    <col min="8" max="8" width="15.77734375" style="7" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" style="7" customWidth="1"/>
+    <col min="10" max="16384" width="18.6640625" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -3175,22 +2685,20 @@
   <sheetPr codeName="工作表2"/>
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18.6328125" defaultRowHeight="17"/>
+  <sheetFormatPr defaultColWidth="18.6640625" defaultRowHeight="16.2"/>
   <cols>
-    <col min="1" max="1" width="10.453125" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.6328125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="16.1796875" style="7" customWidth="1"/>
-    <col min="4" max="4" width="18.36328125" style="7" customWidth="1"/>
-    <col min="5" max="5" width="11.90625" style="7" customWidth="1"/>
+    <col min="1" max="1" width="10.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="16.21875" style="7" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" style="7" customWidth="1"/>
     <col min="6" max="6" width="15" style="7" customWidth="1"/>
-    <col min="7" max="7" width="16.90625" style="7" customWidth="1"/>
-    <col min="8" max="8" width="15.81640625" style="7" customWidth="1"/>
-    <col min="9" max="9" width="13.36328125" style="7" customWidth="1"/>
-    <col min="10" max="16384" width="18.6328125" style="7"/>
+    <col min="7" max="7" width="16.88671875" style="7" customWidth="1"/>
+    <col min="8" max="8" width="15.77734375" style="7" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" style="7" customWidth="1"/>
+    <col min="10" max="16384" width="18.6640625" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -3233,21 +2741,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D88A8D2-3A0B-4501-B8CC-32B64CFDD49F}">
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18.6328125" defaultRowHeight="17"/>
+  <sheetFormatPr defaultColWidth="18.6640625" defaultRowHeight="16.2"/>
   <cols>
-    <col min="1" max="1" width="13.90625" style="7" customWidth="1"/>
+    <col min="1" max="1" width="13.88671875" style="7" customWidth="1"/>
     <col min="2" max="2" width="6" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.1796875" style="7" customWidth="1"/>
-    <col min="4" max="5" width="10.453125" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.21875" style="7" customWidth="1"/>
+    <col min="4" max="5" width="10.44140625" style="7" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" style="7" customWidth="1"/>
-    <col min="7" max="7" width="16.90625" style="7" customWidth="1"/>
-    <col min="8" max="8" width="15.81640625" style="7" customWidth="1"/>
-    <col min="9" max="9" width="13.36328125" style="7" customWidth="1"/>
-    <col min="10" max="16384" width="18.6328125" style="7"/>
+    <col min="7" max="7" width="16.88671875" style="7" customWidth="1"/>
+    <col min="8" max="8" width="15.77734375" style="7" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" style="7" customWidth="1"/>
+    <col min="10" max="16384" width="18.6640625" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -3293,18 +2799,18 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18.6328125" defaultRowHeight="17"/>
+  <sheetFormatPr defaultColWidth="18.6640625" defaultRowHeight="16.2"/>
   <cols>
-    <col min="1" max="1" width="10.453125" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.6328125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="16.1796875" style="7" customWidth="1"/>
-    <col min="4" max="4" width="18.36328125" style="7" customWidth="1"/>
-    <col min="5" max="5" width="11.90625" style="7" customWidth="1"/>
+    <col min="1" max="1" width="10.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="16.21875" style="7" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" style="7" customWidth="1"/>
     <col min="6" max="6" width="15" style="7" customWidth="1"/>
-    <col min="7" max="7" width="16.90625" style="7" customWidth="1"/>
-    <col min="8" max="8" width="15.81640625" style="7" customWidth="1"/>
-    <col min="9" max="9" width="13.36328125" style="7" customWidth="1"/>
-    <col min="10" max="16384" width="18.6328125" style="7"/>
+    <col min="7" max="7" width="16.88671875" style="7" customWidth="1"/>
+    <col min="8" max="8" width="15.77734375" style="7" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" style="7" customWidth="1"/>
+    <col min="10" max="16384" width="18.6640625" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -3347,21 +2853,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51005596-7AF6-4E48-8F14-34158BB9C6E7}">
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18.6328125" defaultRowHeight="17"/>
+  <sheetFormatPr defaultColWidth="18.6640625" defaultRowHeight="16.2"/>
   <cols>
-    <col min="1" max="1" width="13.90625" style="7" customWidth="1"/>
+    <col min="1" max="1" width="13.88671875" style="7" customWidth="1"/>
     <col min="2" max="2" width="6" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.1796875" style="7" customWidth="1"/>
-    <col min="4" max="5" width="10.453125" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.21875" style="7" customWidth="1"/>
+    <col min="4" max="5" width="10.44140625" style="7" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" style="7" customWidth="1"/>
-    <col min="7" max="7" width="16.90625" style="7" customWidth="1"/>
-    <col min="8" max="8" width="15.81640625" style="7" customWidth="1"/>
-    <col min="9" max="9" width="13.36328125" style="7" customWidth="1"/>
-    <col min="10" max="16384" width="18.6328125" style="7"/>
+    <col min="7" max="7" width="16.88671875" style="7" customWidth="1"/>
+    <col min="8" max="8" width="15.77734375" style="7" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" style="7" customWidth="1"/>
+    <col min="10" max="16384" width="18.6640625" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -3408,35 +2912,35 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F9" sqref="F8:F9"/>
+      <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.2"/>
   <cols>
-    <col min="1" max="1" width="8.36328125" style="13" customWidth="1"/>
-    <col min="2" max="2" width="15.81640625" style="9" customWidth="1"/>
-    <col min="3" max="3" width="15.54296875" style="9" customWidth="1"/>
-    <col min="4" max="4" width="11.90625" style="9" customWidth="1"/>
-    <col min="5" max="5" width="16.08984375" style="9" customWidth="1"/>
-    <col min="6" max="6" width="14.81640625" style="9" customWidth="1"/>
-    <col min="7" max="8" width="12.90625" style="9" customWidth="1"/>
-    <col min="9" max="9" width="11.6328125" style="14" customWidth="1"/>
+    <col min="1" max="1" width="8.33203125" style="13" customWidth="1"/>
+    <col min="2" max="2" width="15.77734375" style="9" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" style="9" customWidth="1"/>
+    <col min="4" max="4" width="11.88671875" style="9" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" style="9" customWidth="1"/>
+    <col min="6" max="6" width="14.77734375" style="9" customWidth="1"/>
+    <col min="7" max="8" width="12.88671875" style="9" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" style="14" customWidth="1"/>
     <col min="10" max="10" width="9" style="8"/>
     <col min="11" max="16384" width="9" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="24.75" customHeight="1">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
     </row>
     <row r="2" spans="1:9" ht="24" customHeight="1">
       <c r="A2" s="10" t="s">
@@ -3577,290 +3081,276 @@
   <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J14" sqref="A1:XFD1048576"/>
+      <selection sqref="A1:O1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="9.453125" style="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.453125" style="17" customWidth="1"/>
-    <col min="3" max="3" width="8.08984375" style="17" customWidth="1"/>
-    <col min="4" max="4" width="9" style="17"/>
-    <col min="5" max="5" width="8.36328125" style="17" customWidth="1"/>
-    <col min="6" max="6" width="6.6328125" style="34" customWidth="1"/>
-    <col min="7" max="7" width="8.08984375" style="34" customWidth="1"/>
-    <col min="8" max="8" width="6.6328125" style="34" customWidth="1"/>
-    <col min="9" max="9" width="8.08984375" style="34" customWidth="1"/>
-    <col min="10" max="10" width="6.6328125" style="34" customWidth="1"/>
-    <col min="11" max="11" width="8.08984375" style="34" customWidth="1"/>
-    <col min="12" max="12" width="7.08984375" style="35" customWidth="1"/>
-    <col min="13" max="13" width="8.08984375" style="34" customWidth="1"/>
-    <col min="14" max="14" width="10" style="17" customWidth="1"/>
-    <col min="15" max="15" width="8.08984375" style="36" customWidth="1"/>
-    <col min="16" max="16" width="7.90625" style="17" customWidth="1"/>
-    <col min="17" max="16384" width="9" style="17"/>
+    <col min="1" max="1" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9" style="1"/>
+    <col min="5" max="5" width="8.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="6.6640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="8.109375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="6.6640625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="8.109375" style="3" customWidth="1"/>
+    <col min="10" max="10" width="6.6640625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="8.109375" style="3" customWidth="1"/>
+    <col min="12" max="12" width="7.109375" style="4" customWidth="1"/>
+    <col min="13" max="13" width="8.109375" style="3" customWidth="1"/>
+    <col min="14" max="14" width="10" style="1" customWidth="1"/>
+    <col min="15" max="15" width="8.109375" style="5" customWidth="1"/>
+    <col min="16" max="16" width="7.88671875" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="18.5">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:15" ht="18">
+      <c r="A1" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
     </row>
     <row r="2" spans="1:15" ht="16.5" customHeight="1">
-      <c r="A2" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="18" t="s">
+      <c r="A2" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20" t="s">
+      <c r="G2" s="25"/>
+      <c r="H2" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20" t="s">
+      <c r="I2" s="25"/>
+      <c r="J2" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20" t="s">
+      <c r="K2" s="25"/>
+      <c r="L2" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="M2" s="20"/>
-      <c r="N2" s="21" t="s">
+      <c r="M2" s="25"/>
+      <c r="N2" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="O2" s="22" t="s">
+      <c r="O2" s="29" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="24" customFormat="1">
-      <c r="A3" s="18"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="23" t="s">
+    <row r="3" spans="1:15" s="2" customFormat="1">
+      <c r="A3" s="30"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="G3" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="23" t="s">
+      <c r="H3" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="23" t="s">
+      <c r="I3" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="23" t="s">
+      <c r="J3" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="23" t="s">
+      <c r="K3" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="23" t="s">
+      <c r="L3" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="M3" s="23" t="s">
+      <c r="M3" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="N3" s="21"/>
-      <c r="O3" s="21"/>
+      <c r="N3" s="24"/>
+      <c r="O3" s="24"/>
     </row>
     <row r="4" spans="1:15">
-      <c r="A4" s="25"/>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="28"/>
-      <c r="J4" s="29"/>
-      <c r="K4" s="28"/>
-      <c r="L4" s="29"/>
-      <c r="M4" s="28"/>
-      <c r="N4" s="30"/>
-      <c r="O4" s="26"/>
+      <c r="A4" s="17"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="18"/>
     </row>
     <row r="5" spans="1:15">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="29">
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="21">
         <f t="shared" ref="F5:K5" si="0">SUM(F4:F4)</f>
         <v>0</v>
       </c>
-      <c r="G5" s="29">
+      <c r="G5" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H5" s="29">
+      <c r="H5" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I5" s="28">
+      <c r="I5" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J5" s="29">
+      <c r="J5" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K5" s="29">
+      <c r="K5" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L5" s="29">
+      <c r="L5" s="21">
         <f>F5+H5+J5</f>
         <v>0</v>
       </c>
-      <c r="M5" s="28">
+      <c r="M5" s="20">
         <f>G5+I5+K5</f>
         <v>0</v>
       </c>
-      <c r="N5" s="25"/>
-      <c r="O5" s="31"/>
+      <c r="N5" s="17"/>
+      <c r="O5" s="22"/>
     </row>
     <row r="6" spans="1:15">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="20">
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="25">
         <f>SUBTOTAL(3,$C4:$C4)</f>
         <v>0</v>
       </c>
-      <c r="G6" s="20"/>
-      <c r="H6" s="32">
+      <c r="G6" s="25"/>
+      <c r="H6" s="27">
         <f>SUBTOTAL(3,$C4:$C4)</f>
         <v>0</v>
       </c>
-      <c r="I6" s="32"/>
-      <c r="J6" s="20">
+      <c r="I6" s="27"/>
+      <c r="J6" s="25">
         <f>SUBTOTAL(3,$C4:$C4)</f>
         <v>0</v>
       </c>
-      <c r="K6" s="20"/>
-      <c r="L6" s="20">
+      <c r="K6" s="25"/>
+      <c r="L6" s="25">
         <f>SUBTOTAL(3,$C4:$C4)</f>
         <v>0</v>
       </c>
-      <c r="M6" s="20"/>
-      <c r="N6" s="25"/>
-      <c r="O6" s="31"/>
+      <c r="M6" s="25"/>
+      <c r="N6" s="17"/>
+      <c r="O6" s="22"/>
     </row>
     <row r="7" spans="1:15">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="20">
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="25">
         <f>COUNTIF(F4:F4,"&lt;&gt;0")</f>
         <v>1</v>
       </c>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20">
+      <c r="G7" s="25"/>
+      <c r="H7" s="25">
         <f>COUNTIF(H4:H4,"&lt;&gt;0")</f>
         <v>1</v>
       </c>
-      <c r="I7" s="20"/>
-      <c r="J7" s="20">
+      <c r="I7" s="25"/>
+      <c r="J7" s="25">
         <f>COUNTIF(J4:J4,"&lt;&gt;0")</f>
         <v>1</v>
       </c>
-      <c r="K7" s="20"/>
-      <c r="L7" s="20">
+      <c r="K7" s="25"/>
+      <c r="L7" s="25">
         <f>COUNTIF(L4:L4,"&lt;&gt;0")</f>
         <v>1</v>
       </c>
-      <c r="M7" s="20"/>
-      <c r="N7" s="20"/>
-      <c r="O7" s="20"/>
+      <c r="M7" s="25"/>
+      <c r="N7" s="25"/>
+      <c r="O7" s="25"/>
     </row>
     <row r="8" spans="1:15">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="33" t="e">
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="26" t="e">
         <f>F7/F6</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G8" s="33"/>
-      <c r="H8" s="33" t="e">
+      <c r="G8" s="26"/>
+      <c r="H8" s="26" t="e">
         <f>H7/H6</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I8" s="33"/>
-      <c r="J8" s="33" t="e">
+      <c r="I8" s="26"/>
+      <c r="J8" s="26" t="e">
         <f>J7/J6</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K8" s="33"/>
-      <c r="L8" s="33" t="e">
+      <c r="K8" s="26"/>
+      <c r="L8" s="26" t="e">
         <f>L7/L6</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M8" s="33"/>
-      <c r="N8" s="20"/>
-      <c r="O8" s="20"/>
+      <c r="M8" s="26"/>
+      <c r="N8" s="25"/>
+      <c r="O8" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="J7:K7"/>
     <mergeCell ref="A1:O1"/>
     <mergeCell ref="N8:O8"/>
     <mergeCell ref="J8:K8"/>
@@ -3877,6 +3367,20 @@
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="H8:I8"/>
     <mergeCell ref="A7:E7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="O4">
@@ -3913,500 +3417,279 @@
   <sheetPr codeName="Sheet7">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R17"/>
+  <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R17" sqref="A1:R17"/>
+      <selection sqref="A1:O1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.453125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.08984375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="9" style="1"/>
-    <col min="5" max="5" width="8.36328125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="6.6328125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="8.08984375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="6.6328125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="8.08984375" style="3" customWidth="1"/>
-    <col min="10" max="10" width="6.6328125" style="3" customWidth="1"/>
-    <col min="11" max="11" width="8.08984375" style="3" customWidth="1"/>
-    <col min="12" max="12" width="7.08984375" style="4" customWidth="1"/>
-    <col min="13" max="13" width="8.08984375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="6.6640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="8.109375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="6.6640625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="8.109375" style="3" customWidth="1"/>
+    <col min="10" max="10" width="6.6640625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="8.109375" style="3" customWidth="1"/>
+    <col min="12" max="12" width="7.109375" style="4" customWidth="1"/>
+    <col min="13" max="13" width="8.109375" style="3" customWidth="1"/>
     <col min="14" max="14" width="10" style="1" customWidth="1"/>
-    <col min="15" max="15" width="8.08984375" style="5" customWidth="1"/>
-    <col min="16" max="16" width="7.90625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="8.109375" style="5" customWidth="1"/>
+    <col min="16" max="16" width="7.88671875" style="1" customWidth="1"/>
     <col min="17" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="18.5">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:15" ht="18">
+      <c r="A1" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
-    </row>
-    <row r="2" spans="1:18" ht="16.5" customHeight="1">
-      <c r="A2" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="18" t="s">
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+    </row>
+    <row r="2" spans="1:15" ht="16.5" customHeight="1">
+      <c r="A2" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20" t="s">
+      <c r="G2" s="25"/>
+      <c r="H2" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20" t="s">
+      <c r="I2" s="25"/>
+      <c r="J2" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20" t="s">
+      <c r="K2" s="25"/>
+      <c r="L2" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="M2" s="20"/>
-      <c r="N2" s="21" t="s">
+      <c r="M2" s="25"/>
+      <c r="N2" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="O2" s="22" t="s">
+      <c r="O2" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="P2" s="17"/>
-      <c r="Q2" s="17"/>
-      <c r="R2" s="17"/>
-    </row>
-    <row r="3" spans="1:18" s="2" customFormat="1">
-      <c r="A3" s="18"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="23" t="s">
+    </row>
+    <row r="3" spans="1:15" s="2" customFormat="1">
+      <c r="A3" s="30"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="G3" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="23" t="s">
+      <c r="H3" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="23" t="s">
+      <c r="I3" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="23" t="s">
+      <c r="J3" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="23" t="s">
+      <c r="K3" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="23" t="s">
+      <c r="L3" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="M3" s="23" t="s">
+      <c r="M3" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="21"/>
-      <c r="O3" s="21"/>
-      <c r="P3" s="24"/>
-      <c r="Q3" s="24"/>
-      <c r="R3" s="24"/>
-    </row>
-    <row r="4" spans="1:18">
-      <c r="A4" s="25"/>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="28"/>
-      <c r="J4" s="29"/>
-      <c r="K4" s="28"/>
-      <c r="L4" s="29"/>
-      <c r="M4" s="28"/>
-      <c r="N4" s="30"/>
-      <c r="O4" s="26"/>
-      <c r="P4" s="17"/>
-      <c r="Q4" s="17"/>
-      <c r="R4" s="17"/>
-    </row>
-    <row r="5" spans="1:18">
-      <c r="A5" s="21" t="s">
+      <c r="N3" s="24"/>
+      <c r="O3" s="24"/>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" s="17"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="18"/>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="29">
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="21">
         <f t="shared" ref="F5:K5" si="0">SUM(F4:F4)</f>
         <v>0</v>
       </c>
-      <c r="G5" s="29">
+      <c r="G5" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H5" s="29">
+      <c r="H5" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I5" s="28">
+      <c r="I5" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J5" s="29">
+      <c r="J5" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K5" s="29">
+      <c r="K5" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L5" s="29">
+      <c r="L5" s="21">
         <f>F5+H5+J5</f>
         <v>0</v>
       </c>
-      <c r="M5" s="28">
+      <c r="M5" s="20">
         <f>G5+I5+K5</f>
         <v>0</v>
       </c>
-      <c r="N5" s="25"/>
-      <c r="O5" s="31"/>
-      <c r="P5" s="17"/>
-      <c r="Q5" s="17"/>
-      <c r="R5" s="17"/>
-    </row>
-    <row r="6" spans="1:18">
-      <c r="A6" s="21" t="s">
+      <c r="N5" s="17"/>
+      <c r="O5" s="22"/>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="20">
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="25">
         <f>SUBTOTAL(3,$C4:$C4)</f>
         <v>0</v>
       </c>
-      <c r="G6" s="20"/>
-      <c r="H6" s="32">
+      <c r="G6" s="25"/>
+      <c r="H6" s="27">
         <f>SUBTOTAL(3,$C4:$C4)</f>
         <v>0</v>
       </c>
-      <c r="I6" s="32"/>
-      <c r="J6" s="20">
+      <c r="I6" s="27"/>
+      <c r="J6" s="25">
         <f>SUBTOTAL(3,$C4:$C4)</f>
         <v>0</v>
       </c>
-      <c r="K6" s="20"/>
-      <c r="L6" s="20">
+      <c r="K6" s="25"/>
+      <c r="L6" s="25">
         <f>SUBTOTAL(3,$C4:$C4)</f>
         <v>0</v>
       </c>
-      <c r="M6" s="20"/>
-      <c r="N6" s="25"/>
-      <c r="O6" s="31"/>
-      <c r="P6" s="17"/>
-      <c r="Q6" s="17"/>
-      <c r="R6" s="17"/>
-    </row>
-    <row r="7" spans="1:18">
-      <c r="A7" s="21" t="s">
+      <c r="M6" s="25"/>
+      <c r="N6" s="17"/>
+      <c r="O6" s="22"/>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="20">
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="25">
         <f>COUNTIF(F4:F4,"&lt;&gt;0")</f>
         <v>1</v>
       </c>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20">
+      <c r="G7" s="25"/>
+      <c r="H7" s="25">
         <f>COUNTIF(H4:H4,"&lt;&gt;0")</f>
         <v>1</v>
       </c>
-      <c r="I7" s="20"/>
-      <c r="J7" s="20">
+      <c r="I7" s="25"/>
+      <c r="J7" s="25">
         <f>COUNTIF(J4:J4,"&lt;&gt;0")</f>
         <v>1</v>
       </c>
-      <c r="K7" s="20"/>
-      <c r="L7" s="20">
+      <c r="K7" s="25"/>
+      <c r="L7" s="25">
         <f>COUNTIF(L4:L4,"&lt;&gt;0")</f>
         <v>1</v>
       </c>
-      <c r="M7" s="20"/>
-      <c r="N7" s="20"/>
-      <c r="O7" s="20"/>
-      <c r="P7" s="17"/>
-      <c r="Q7" s="17"/>
-      <c r="R7" s="17"/>
-    </row>
-    <row r="8" spans="1:18">
-      <c r="A8" s="21" t="s">
+      <c r="M7" s="25"/>
+      <c r="N7" s="25"/>
+      <c r="O7" s="25"/>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="33" t="e">
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="26" t="e">
         <f>F7/F6</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G8" s="33"/>
-      <c r="H8" s="33" t="e">
+      <c r="G8" s="26"/>
+      <c r="H8" s="26" t="e">
         <f>H7/H6</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I8" s="33"/>
-      <c r="J8" s="33" t="e">
+      <c r="I8" s="26"/>
+      <c r="J8" s="26" t="e">
         <f>J7/J6</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K8" s="33"/>
-      <c r="L8" s="33" t="e">
+      <c r="K8" s="26"/>
+      <c r="L8" s="26" t="e">
         <f>L7/L6</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M8" s="33"/>
-      <c r="N8" s="20"/>
-      <c r="O8" s="20"/>
-      <c r="P8" s="17"/>
-      <c r="Q8" s="17"/>
-      <c r="R8" s="17"/>
-    </row>
-    <row r="9" spans="1:18">
-      <c r="A9" s="17"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="34"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="34"/>
-      <c r="J9" s="34"/>
-      <c r="K9" s="34"/>
-      <c r="L9" s="35"/>
-      <c r="M9" s="34"/>
-      <c r="N9" s="17"/>
-      <c r="O9" s="36"/>
-      <c r="P9" s="17"/>
-      <c r="Q9" s="17"/>
-      <c r="R9" s="17"/>
-    </row>
-    <row r="10" spans="1:18">
-      <c r="A10" s="17"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="34"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="34"/>
-      <c r="J10" s="34"/>
-      <c r="K10" s="34"/>
-      <c r="L10" s="35"/>
-      <c r="M10" s="34"/>
-      <c r="N10" s="17"/>
-      <c r="O10" s="36"/>
-      <c r="P10" s="17"/>
-      <c r="Q10" s="17"/>
-      <c r="R10" s="17"/>
-    </row>
-    <row r="11" spans="1:18">
-      <c r="A11" s="17"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="34"/>
-      <c r="J11" s="34"/>
-      <c r="K11" s="34"/>
-      <c r="L11" s="35"/>
-      <c r="M11" s="34"/>
-      <c r="N11" s="17"/>
-      <c r="O11" s="36"/>
-      <c r="P11" s="17"/>
-      <c r="Q11" s="17"/>
-      <c r="R11" s="17"/>
-    </row>
-    <row r="12" spans="1:18">
-      <c r="A12" s="17"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="34"/>
-      <c r="J12" s="34"/>
-      <c r="K12" s="34"/>
-      <c r="L12" s="35"/>
-      <c r="M12" s="34"/>
-      <c r="N12" s="17"/>
-      <c r="O12" s="36"/>
-      <c r="P12" s="17"/>
-      <c r="Q12" s="17"/>
-      <c r="R12" s="17"/>
-    </row>
-    <row r="13" spans="1:18">
-      <c r="A13" s="17"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="34"/>
-      <c r="G13" s="34"/>
-      <c r="H13" s="34"/>
-      <c r="I13" s="34"/>
-      <c r="J13" s="34"/>
-      <c r="K13" s="34"/>
-      <c r="L13" s="35"/>
-      <c r="M13" s="34"/>
-      <c r="N13" s="17"/>
-      <c r="O13" s="36"/>
-      <c r="P13" s="17"/>
-      <c r="Q13" s="17"/>
-      <c r="R13" s="17"/>
-    </row>
-    <row r="14" spans="1:18">
-      <c r="A14" s="17"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="34"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="34"/>
-      <c r="J14" s="34"/>
-      <c r="K14" s="34"/>
-      <c r="L14" s="35"/>
-      <c r="M14" s="34"/>
-      <c r="N14" s="17"/>
-      <c r="O14" s="36"/>
-      <c r="P14" s="17"/>
-      <c r="Q14" s="17"/>
-      <c r="R14" s="17"/>
-    </row>
-    <row r="15" spans="1:18">
-      <c r="A15" s="17"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="34"/>
-      <c r="J15" s="34"/>
-      <c r="K15" s="34"/>
-      <c r="L15" s="35"/>
-      <c r="M15" s="34"/>
-      <c r="N15" s="17"/>
-      <c r="O15" s="36"/>
-      <c r="P15" s="17"/>
-      <c r="Q15" s="17"/>
-      <c r="R15" s="17"/>
-    </row>
-    <row r="16" spans="1:18">
-      <c r="A16" s="17"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="34"/>
-      <c r="J16" s="34"/>
-      <c r="K16" s="34"/>
-      <c r="L16" s="35"/>
-      <c r="M16" s="34"/>
-      <c r="N16" s="17"/>
-      <c r="O16" s="36"/>
-      <c r="P16" s="17"/>
-      <c r="Q16" s="17"/>
-      <c r="R16" s="17"/>
-    </row>
-    <row r="17" spans="1:18">
-      <c r="A17" s="17"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="34"/>
-      <c r="G17" s="34"/>
-      <c r="H17" s="34"/>
-      <c r="I17" s="34"/>
-      <c r="J17" s="34"/>
-      <c r="K17" s="34"/>
-      <c r="L17" s="35"/>
-      <c r="M17" s="34"/>
-      <c r="N17" s="17"/>
-      <c r="O17" s="36"/>
-      <c r="P17" s="17"/>
-      <c r="Q17" s="17"/>
-      <c r="R17" s="17"/>
+      <c r="M8" s="26"/>
+      <c r="N8" s="25"/>
+      <c r="O8" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="A1:O1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="O2:O3"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
     <mergeCell ref="L6:M6"/>
     <mergeCell ref="N8:O8"/>
     <mergeCell ref="A7:E7"/>
@@ -4420,6 +3703,23 @@
     <mergeCell ref="H8:I8"/>
     <mergeCell ref="J8:K8"/>
     <mergeCell ref="L8:M8"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="O2:O3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="O4">

</xml_diff>

<commit_message>
Auto-committed on 2023/09/15 週五 17:07:32.90
</commit_message>
<xml_diff>
--- a/Program/Other/LP005_底稿_協辦考核核算.xlsx
+++ b/Program/Other/LP005_底稿_協辦考核核算.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LINDA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SVN\SKL\iTX\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ED53644-2E2C-4D20-9DC9-261CC87C7A62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="791" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="791" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="1月件數" sheetId="70" r:id="rId1"/>
@@ -145,12 +144,12 @@
     <definedName name="金額9月數字" localSheetId="11">#REF!</definedName>
     <definedName name="金額9月數字">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="53">
   <si>
     <r>
       <rPr>
@@ -673,11 +672,15 @@
     <t>計件代碼</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>備註</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="0.0%"/>
@@ -910,7 +913,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -919,14 +922,11 @@
     <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -934,12 +934,15 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="177" fontId="10" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
-    <cellStyle name="一般 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="一般_9804" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="千分位 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="一般 2" xfId="1"/>
+    <cellStyle name="一般_9804" xfId="2"/>
+    <cellStyle name="千分位 2" xfId="3"/>
   </cellStyles>
   <dxfs count="60">
     <dxf>
@@ -1722,11 +1725,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0869A94A-3298-4599-A82F-79706276E934}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="工作表1"/>
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.6640625" defaultRowHeight="16.2"/>
   <cols>
@@ -1779,7 +1782,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E4B404D-2551-48A5-95C3-F293796C9D12}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet8">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -1811,38 +1814,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
     </row>
     <row r="2" spans="1:15" ht="16.5" customHeight="1">
-      <c r="A2" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="30" t="s">
+      <c r="A2" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="30" t="s">
+      <c r="D2" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="31" t="s">
+      <c r="E2" s="30" t="s">
         <v>27</v>
       </c>
       <c r="F2" s="25" t="s">
@@ -1861,19 +1864,19 @@
         <v>7</v>
       </c>
       <c r="M2" s="25"/>
-      <c r="N2" s="24" t="s">
+      <c r="N2" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="O2" s="29" t="s">
+      <c r="O2" s="27" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:15" s="2" customFormat="1">
-      <c r="A3" s="30"/>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
+      <c r="A3" s="29"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
       <c r="F3" s="16" t="s">
         <v>11</v>
       </c>
@@ -1898,8 +1901,8 @@
       <c r="M3" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="24"/>
-      <c r="O3" s="24"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="28"/>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" s="17"/>
@@ -1919,13 +1922,13 @@
       <c r="O4" s="18"/>
     </row>
     <row r="5" spans="1:15">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
       <c r="F5" s="21">
         <f t="shared" ref="F5:K5" si="0">SUM(F4:F4)</f>
         <v>0</v>
@@ -1962,23 +1965,23 @@
       <c r="O5" s="22"/>
     </row>
     <row r="6" spans="1:15">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
       <c r="F6" s="25">
         <f>SUBTOTAL(3,$C4:$C4)</f>
         <v>0</v>
       </c>
       <c r="G6" s="25"/>
-      <c r="H6" s="27">
+      <c r="H6" s="31">
         <f>SUBTOTAL(3,$C4:$C4)</f>
         <v>0</v>
       </c>
-      <c r="I6" s="27"/>
+      <c r="I6" s="31"/>
       <c r="J6" s="25">
         <f>SUBTOTAL(3,$C4:$C4)</f>
         <v>0</v>
@@ -1993,13 +1996,13 @@
       <c r="O6" s="22"/>
     </row>
     <row r="7" spans="1:15">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="24"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
       <c r="F7" s="25">
         <f>COUNTIF(F4:F4,"&lt;&gt;0")</f>
         <v>1</v>
@@ -2024,13 +2027,13 @@
       <c r="O7" s="25"/>
     </row>
     <row r="8" spans="1:15">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="24"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
       <c r="F8" s="26" t="e">
         <f>F7/F6</f>
         <v>#DIV/0!</v>
@@ -2056,6 +2059,23 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="O2:O3"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:K6"/>
     <mergeCell ref="L6:M6"/>
     <mergeCell ref="N8:O8"/>
     <mergeCell ref="A7:E7"/>
@@ -2069,23 +2089,6 @@
     <mergeCell ref="H8:I8"/>
     <mergeCell ref="J8:K8"/>
     <mergeCell ref="L8:M8"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="A1:O1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="O2:O3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="O4">
@@ -2118,7 +2121,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BA84D84-784A-4975-B6C9-64841D457C59}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet9">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -2150,38 +2153,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
     </row>
     <row r="2" spans="1:15" ht="16.5" customHeight="1">
-      <c r="A2" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="30" t="s">
+      <c r="A2" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="30" t="s">
+      <c r="D2" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="31" t="s">
+      <c r="E2" s="30" t="s">
         <v>27</v>
       </c>
       <c r="F2" s="25" t="s">
@@ -2200,19 +2203,19 @@
         <v>7</v>
       </c>
       <c r="M2" s="25"/>
-      <c r="N2" s="24" t="s">
+      <c r="N2" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="O2" s="29" t="s">
+      <c r="O2" s="27" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:15" s="2" customFormat="1">
-      <c r="A3" s="30"/>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
+      <c r="A3" s="29"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
       <c r="F3" s="16" t="s">
         <v>11</v>
       </c>
@@ -2237,8 +2240,8 @@
       <c r="M3" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="24"/>
-      <c r="O3" s="24"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="28"/>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" s="17"/>
@@ -2258,13 +2261,13 @@
       <c r="O4" s="18"/>
     </row>
     <row r="5" spans="1:15">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
       <c r="F5" s="21">
         <f t="shared" ref="F5:K5" si="0">SUM(F4:F4)</f>
         <v>0</v>
@@ -2301,23 +2304,23 @@
       <c r="O5" s="22"/>
     </row>
     <row r="6" spans="1:15">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
       <c r="F6" s="25">
         <f>SUBTOTAL(3,$C4:$C4)</f>
         <v>0</v>
       </c>
       <c r="G6" s="25"/>
-      <c r="H6" s="27">
+      <c r="H6" s="31">
         <f>SUBTOTAL(3,$C4:$C4)</f>
         <v>0</v>
       </c>
-      <c r="I6" s="27"/>
+      <c r="I6" s="31"/>
       <c r="J6" s="25">
         <f>SUBTOTAL(3,$C4:$C4)</f>
         <v>0</v>
@@ -2332,13 +2335,13 @@
       <c r="O6" s="22"/>
     </row>
     <row r="7" spans="1:15">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="24"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
       <c r="F7" s="25">
         <f>COUNTIF(F4:F4,"&lt;&gt;0")</f>
         <v>1</v>
@@ -2363,13 +2366,13 @@
       <c r="O7" s="25"/>
     </row>
     <row r="8" spans="1:15">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="24"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
       <c r="F8" s="26" t="e">
         <f>F7/F6</f>
         <v>#DIV/0!</v>
@@ -2395,6 +2398,23 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="O2:O3"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:K6"/>
     <mergeCell ref="L6:M6"/>
     <mergeCell ref="N8:O8"/>
     <mergeCell ref="A7:E7"/>
@@ -2408,23 +2428,6 @@
     <mergeCell ref="H8:I8"/>
     <mergeCell ref="J8:K8"/>
     <mergeCell ref="L8:M8"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="A1:O1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="O2:O3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="O4">
@@ -2457,7 +2460,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="工作表5">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
@@ -2626,7 +2629,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F5A011B-B6C8-45CD-9219-0AEAA3A08C8A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2681,7 +2684,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F766160-E095-4118-B54A-2F77E016B710}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="工作表2"/>
   <dimension ref="A1:I1"/>
   <sheetViews>
@@ -2738,7 +2741,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D88A8D2-3A0B-4501-B8CC-32B64CFDD49F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2793,7 +2796,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8E5C2AE-C013-44A5-A6CC-1F4406CBE6E1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="工作表3"/>
   <dimension ref="A1:I1"/>
   <sheetViews>
@@ -2850,7 +2853,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51005596-7AF6-4E48-8F14-34158BB9C6E7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2905,14 +2908,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54875884-19B4-4CF5-B76F-57B5FDB4F146}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="工作表4">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:I1"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.2"/>
@@ -2968,7 +2971,7 @@
         <v>38</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="18.899999999999999" customHeight="1">
@@ -3074,7 +3077,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet6">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -3106,38 +3109,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
     </row>
     <row r="2" spans="1:15" ht="16.5" customHeight="1">
-      <c r="A2" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="30" t="s">
+      <c r="A2" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="30" t="s">
+      <c r="D2" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="31" t="s">
+      <c r="E2" s="30" t="s">
         <v>27</v>
       </c>
       <c r="F2" s="25" t="s">
@@ -3156,19 +3159,19 @@
         <v>19</v>
       </c>
       <c r="M2" s="25"/>
-      <c r="N2" s="24" t="s">
+      <c r="N2" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="O2" s="29" t="s">
+      <c r="O2" s="27" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:15" s="2" customFormat="1">
-      <c r="A3" s="30"/>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
+      <c r="A3" s="29"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
       <c r="F3" s="16" t="s">
         <v>22</v>
       </c>
@@ -3193,8 +3196,8 @@
       <c r="M3" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="N3" s="24"/>
-      <c r="O3" s="24"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="28"/>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" s="17"/>
@@ -3214,13 +3217,13 @@
       <c r="O4" s="18"/>
     </row>
     <row r="5" spans="1:15">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
       <c r="F5" s="21">
         <f t="shared" ref="F5:K5" si="0">SUM(F4:F4)</f>
         <v>0</v>
@@ -3257,23 +3260,23 @@
       <c r="O5" s="22"/>
     </row>
     <row r="6" spans="1:15">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
       <c r="F6" s="25">
         <f>SUBTOTAL(3,$C4:$C4)</f>
         <v>0</v>
       </c>
       <c r="G6" s="25"/>
-      <c r="H6" s="27">
+      <c r="H6" s="31">
         <f>SUBTOTAL(3,$C4:$C4)</f>
         <v>0</v>
       </c>
-      <c r="I6" s="27"/>
+      <c r="I6" s="31"/>
       <c r="J6" s="25">
         <f>SUBTOTAL(3,$C4:$C4)</f>
         <v>0</v>
@@ -3288,13 +3291,13 @@
       <c r="O6" s="22"/>
     </row>
     <row r="7" spans="1:15">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="24"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
       <c r="F7" s="25">
         <f>COUNTIF(F4:F4,"&lt;&gt;0")</f>
         <v>1</v>
@@ -3319,13 +3322,13 @@
       <c r="O7" s="25"/>
     </row>
     <row r="8" spans="1:15">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="24"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
       <c r="F8" s="26" t="e">
         <f>F7/F6</f>
         <v>#DIV/0!</v>
@@ -3351,6 +3354,20 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="J7:K7"/>
     <mergeCell ref="A1:O1"/>
     <mergeCell ref="N8:O8"/>
     <mergeCell ref="J8:K8"/>
@@ -3367,20 +3384,6 @@
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="H8:I8"/>
     <mergeCell ref="A7:E7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="O4">
@@ -3413,7 +3416,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E7C8C0C-9802-4F23-8AB8-CE879F636DF6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet7">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -3445,38 +3448,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
     </row>
     <row r="2" spans="1:15" ht="16.5" customHeight="1">
-      <c r="A2" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="30" t="s">
+      <c r="A2" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="30" t="s">
+      <c r="D2" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="31" t="s">
+      <c r="E2" s="30" t="s">
         <v>27</v>
       </c>
       <c r="F2" s="25" t="s">
@@ -3495,19 +3498,19 @@
         <v>7</v>
       </c>
       <c r="M2" s="25"/>
-      <c r="N2" s="24" t="s">
+      <c r="N2" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="O2" s="29" t="s">
+      <c r="O2" s="27" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:15" s="2" customFormat="1">
-      <c r="A3" s="30"/>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
+      <c r="A3" s="29"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
       <c r="F3" s="16" t="s">
         <v>11</v>
       </c>
@@ -3532,8 +3535,8 @@
       <c r="M3" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="24"/>
-      <c r="O3" s="24"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="28"/>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" s="17"/>
@@ -3553,13 +3556,13 @@
       <c r="O4" s="18"/>
     </row>
     <row r="5" spans="1:15">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
       <c r="F5" s="21">
         <f t="shared" ref="F5:K5" si="0">SUM(F4:F4)</f>
         <v>0</v>
@@ -3596,23 +3599,23 @@
       <c r="O5" s="22"/>
     </row>
     <row r="6" spans="1:15">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
       <c r="F6" s="25">
         <f>SUBTOTAL(3,$C4:$C4)</f>
         <v>0</v>
       </c>
       <c r="G6" s="25"/>
-      <c r="H6" s="27">
+      <c r="H6" s="31">
         <f>SUBTOTAL(3,$C4:$C4)</f>
         <v>0</v>
       </c>
-      <c r="I6" s="27"/>
+      <c r="I6" s="31"/>
       <c r="J6" s="25">
         <f>SUBTOTAL(3,$C4:$C4)</f>
         <v>0</v>
@@ -3627,13 +3630,13 @@
       <c r="O6" s="22"/>
     </row>
     <row r="7" spans="1:15">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="24"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
       <c r="F7" s="25">
         <f>COUNTIF(F4:F4,"&lt;&gt;0")</f>
         <v>1</v>
@@ -3658,13 +3661,13 @@
       <c r="O7" s="25"/>
     </row>
     <row r="8" spans="1:15">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="24"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
       <c r="F8" s="26" t="e">
         <f>F7/F6</f>
         <v>#DIV/0!</v>
@@ -3690,6 +3693,23 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="O2:O3"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:K6"/>
     <mergeCell ref="L6:M6"/>
     <mergeCell ref="N8:O8"/>
     <mergeCell ref="A7:E7"/>
@@ -3703,23 +3723,6 @@
     <mergeCell ref="H8:I8"/>
     <mergeCell ref="J8:K8"/>
     <mergeCell ref="L8:M8"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="A1:O1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="O2:O3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="O4">

</xml_diff>

<commit_message>
Auto-committed on 2023/09/23 週六 17:09:02.85
</commit_message>
<xml_diff>
--- a/Program/Other/LP005_底稿_協辦考核核算.xlsx
+++ b/Program/Other/LP005_底稿_協辦考核核算.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SVN\SKL\iTX\Other\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SKL_SVN\iTX\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A52867C-E3A3-4AE3-BA77-E6F92BCA91CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="791" activeTab="6"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="791" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1月件數" sheetId="70" r:id="rId1"/>
@@ -144,7 +145,7 @@
     <definedName name="金額9月數字" localSheetId="11">#REF!</definedName>
     <definedName name="金額9月數字">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -680,7 +681,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="0.0%"/>
@@ -840,7 +841,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -913,38 +914,44 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="10" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
-    <cellStyle name="一般 2" xfId="1"/>
-    <cellStyle name="一般_9804" xfId="2"/>
-    <cellStyle name="千分位 2" xfId="3"/>
+    <cellStyle name="一般 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="一般_9804" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="千分位 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
-  <dxfs count="60">
+  <dxfs count="42">
     <dxf>
       <font>
         <condense val="0"/>
@@ -968,21 +975,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF002060"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0000FF"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <condense val="0"/>
         <extend val="0"/>
         <color indexed="10"/>
@@ -1004,6 +996,21 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF002060"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF0000FF"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <condense val="0"/>
         <extend val="0"/>
         <color indexed="10"/>
@@ -1025,21 +1032,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF002060"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0000FF"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <condense val="0"/>
         <extend val="0"/>
         <color indexed="10"/>
@@ -1056,7 +1048,7 @@
       <font>
         <condense val="0"/>
         <extend val="0"/>
-        <color auto="1"/>
+        <color indexed="8"/>
       </font>
     </dxf>
     <dxf>
@@ -1077,7 +1069,7 @@
       <font>
         <condense val="0"/>
         <extend val="0"/>
-        <color indexed="8"/>
+        <color auto="1"/>
       </font>
     </dxf>
     <dxf>
@@ -1098,7 +1090,7 @@
       <font>
         <condense val="0"/>
         <extend val="0"/>
-        <color auto="1"/>
+        <color indexed="8"/>
       </font>
     </dxf>
     <dxf>
@@ -1119,7 +1111,7 @@
       <font>
         <condense val="0"/>
         <extend val="0"/>
-        <color indexed="8"/>
+        <color auto="1"/>
       </font>
     </dxf>
     <dxf>
@@ -1140,7 +1132,7 @@
       <font>
         <condense val="0"/>
         <extend val="0"/>
-        <color auto="1"/>
+        <color indexed="8"/>
       </font>
     </dxf>
     <dxf>
@@ -1161,7 +1153,7 @@
       <font>
         <condense val="0"/>
         <extend val="0"/>
-        <color indexed="8"/>
+        <color auto="1"/>
       </font>
     </dxf>
     <dxf>
@@ -1182,7 +1174,7 @@
       <font>
         <condense val="0"/>
         <extend val="0"/>
-        <color auto="1"/>
+        <color indexed="8"/>
       </font>
     </dxf>
     <dxf>
@@ -1203,7 +1195,7 @@
       <font>
         <condense val="0"/>
         <extend val="0"/>
-        <color indexed="8"/>
+        <color auto="1"/>
       </font>
     </dxf>
     <dxf>
@@ -1229,27 +1221,6 @@
     </dxf>
     <dxf>
       <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF002060"/>
       </font>
     </dxf>
@@ -1261,84 +1232,6 @@
     <dxf>
       <font>
         <color rgb="FF0000FF"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF002060"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0000FF"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color auto="1"/>
       </font>
     </dxf>
   </dxfs>
@@ -1725,7 +1618,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="工作表1"/>
   <dimension ref="A1:I1"/>
   <sheetViews>
@@ -1782,7 +1675,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr codeName="Sheet8">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -1814,38 +1707,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="24"/>
-      <c r="O1" s="24"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
     </row>
     <row r="2" spans="1:15" ht="16.5" customHeight="1">
-      <c r="A2" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="29" t="s">
+      <c r="A2" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="30" t="s">
+      <c r="E2" s="31" t="s">
         <v>27</v>
       </c>
       <c r="F2" s="25" t="s">
@@ -1864,19 +1757,19 @@
         <v>7</v>
       </c>
       <c r="M2" s="25"/>
-      <c r="N2" s="28" t="s">
+      <c r="N2" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="O2" s="27" t="s">
+      <c r="O2" s="29" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:15" s="2" customFormat="1">
-      <c r="A3" s="29"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
+      <c r="A3" s="30"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
       <c r="F3" s="16" t="s">
         <v>11</v>
       </c>
@@ -1901,8 +1794,8 @@
       <c r="M3" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="28"/>
-      <c r="O3" s="28"/>
+      <c r="N3" s="24"/>
+      <c r="O3" s="24"/>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" s="17"/>
@@ -1922,13 +1815,13 @@
       <c r="O4" s="18"/>
     </row>
     <row r="5" spans="1:15">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
       <c r="F5" s="21">
         <f t="shared" ref="F5:K5" si="0">SUM(F4:F4)</f>
         <v>0</v>
@@ -1965,23 +1858,23 @@
       <c r="O5" s="22"/>
     </row>
     <row r="6" spans="1:15">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
       <c r="F6" s="25">
         <f>SUBTOTAL(3,$C4:$C4)</f>
         <v>0</v>
       </c>
       <c r="G6" s="25"/>
-      <c r="H6" s="31">
+      <c r="H6" s="27">
         <f>SUBTOTAL(3,$C4:$C4)</f>
         <v>0</v>
       </c>
-      <c r="I6" s="31"/>
+      <c r="I6" s="27"/>
       <c r="J6" s="25">
         <f>SUBTOTAL(3,$C4:$C4)</f>
         <v>0</v>
@@ -1996,13 +1889,13 @@
       <c r="O6" s="22"/>
     </row>
     <row r="7" spans="1:15">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
       <c r="F7" s="25">
         <f>COUNTIF(F4:F4,"&lt;&gt;0")</f>
         <v>1</v>
@@ -2027,13 +1920,13 @@
       <c r="O7" s="25"/>
     </row>
     <row r="8" spans="1:15">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
       <c r="F8" s="26" t="e">
         <f>F7/F6</f>
         <v>#DIV/0!</v>
@@ -2059,23 +1952,6 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="A1:O1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="O2:O3"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
     <mergeCell ref="L6:M6"/>
     <mergeCell ref="N8:O8"/>
     <mergeCell ref="A7:E7"/>
@@ -2089,27 +1965,44 @@
     <mergeCell ref="H8:I8"/>
     <mergeCell ref="J8:K8"/>
     <mergeCell ref="L8:M8"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="O2:O3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="E4">
+    <cfRule type="cellIs" dxfId="20" priority="4" stopIfTrue="1" operator="equal">
+      <formula>"初級"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="5" stopIfTrue="1" operator="equal">
+      <formula>"中級"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="6" stopIfTrue="1" operator="equal">
+      <formula>"高級"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="O4">
-    <cfRule type="cellIs" dxfId="29" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="1" stopIfTrue="1" operator="equal">
       <formula>"初級"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="2" stopIfTrue="1" operator="equal">
       <formula>"中級"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="3" stopIfTrue="1" operator="equal">
-      <formula>"高級"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E4">
-    <cfRule type="cellIs" dxfId="26" priority="4" stopIfTrue="1" operator="equal">
-      <formula>"初級"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="5" stopIfTrue="1" operator="equal">
-      <formula>"中級"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="3" stopIfTrue="1" operator="equal">
       <formula>"高級"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2121,7 +2014,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr codeName="Sheet9">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -2153,38 +2046,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="24"/>
-      <c r="O1" s="24"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
     </row>
     <row r="2" spans="1:15" ht="16.5" customHeight="1">
-      <c r="A2" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="29" t="s">
+      <c r="A2" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="30" t="s">
+      <c r="E2" s="31" t="s">
         <v>27</v>
       </c>
       <c r="F2" s="25" t="s">
@@ -2203,19 +2096,19 @@
         <v>7</v>
       </c>
       <c r="M2" s="25"/>
-      <c r="N2" s="28" t="s">
+      <c r="N2" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="O2" s="27" t="s">
+      <c r="O2" s="29" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:15" s="2" customFormat="1">
-      <c r="A3" s="29"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
+      <c r="A3" s="30"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
       <c r="F3" s="16" t="s">
         <v>11</v>
       </c>
@@ -2240,8 +2133,8 @@
       <c r="M3" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="28"/>
-      <c r="O3" s="28"/>
+      <c r="N3" s="24"/>
+      <c r="O3" s="24"/>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" s="17"/>
@@ -2261,13 +2154,13 @@
       <c r="O4" s="18"/>
     </row>
     <row r="5" spans="1:15">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
       <c r="F5" s="21">
         <f t="shared" ref="F5:K5" si="0">SUM(F4:F4)</f>
         <v>0</v>
@@ -2304,23 +2197,23 @@
       <c r="O5" s="22"/>
     </row>
     <row r="6" spans="1:15">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
       <c r="F6" s="25">
         <f>SUBTOTAL(3,$C4:$C4)</f>
         <v>0</v>
       </c>
       <c r="G6" s="25"/>
-      <c r="H6" s="31">
+      <c r="H6" s="27">
         <f>SUBTOTAL(3,$C4:$C4)</f>
         <v>0</v>
       </c>
-      <c r="I6" s="31"/>
+      <c r="I6" s="27"/>
       <c r="J6" s="25">
         <f>SUBTOTAL(3,$C4:$C4)</f>
         <v>0</v>
@@ -2335,13 +2228,13 @@
       <c r="O6" s="22"/>
     </row>
     <row r="7" spans="1:15">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
       <c r="F7" s="25">
         <f>COUNTIF(F4:F4,"&lt;&gt;0")</f>
         <v>1</v>
@@ -2366,13 +2259,13 @@
       <c r="O7" s="25"/>
     </row>
     <row r="8" spans="1:15">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
       <c r="F8" s="26" t="e">
         <f>F7/F6</f>
         <v>#DIV/0!</v>
@@ -2398,23 +2291,6 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="A1:O1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="O2:O3"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
     <mergeCell ref="L6:M6"/>
     <mergeCell ref="N8:O8"/>
     <mergeCell ref="A7:E7"/>
@@ -2428,27 +2304,44 @@
     <mergeCell ref="H8:I8"/>
     <mergeCell ref="J8:K8"/>
     <mergeCell ref="L8:M8"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="O2:O3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="E4">
+    <cfRule type="cellIs" dxfId="14" priority="4" stopIfTrue="1" operator="equal">
+      <formula>"初級"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="5" stopIfTrue="1" operator="equal">
+      <formula>"中級"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="6" stopIfTrue="1" operator="equal">
+      <formula>"高級"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="O4">
-    <cfRule type="cellIs" dxfId="23" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="1" stopIfTrue="1" operator="equal">
       <formula>"初級"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="2" stopIfTrue="1" operator="equal">
       <formula>"中級"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="3" stopIfTrue="1" operator="equal">
-      <formula>"高級"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E4">
-    <cfRule type="cellIs" dxfId="20" priority="4" stopIfTrue="1" operator="equal">
-      <formula>"初級"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="5" stopIfTrue="1" operator="equal">
-      <formula>"中級"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="3" stopIfTrue="1" operator="equal">
       <formula>"高級"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2460,14 +2353,14 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr codeName="工作表5">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:I1"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.2"/>
@@ -2553,62 +2446,27 @@
     <mergeCell ref="A1:I1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="G3:H3">
-    <cfRule type="cellIs" dxfId="17" priority="52" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="G3:H4">
+    <cfRule type="cellIs" dxfId="8" priority="4" stopIfTrue="1" operator="equal">
+      <formula>"中級"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="5" stopIfTrue="1" operator="equal">
+      <formula>"高級"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="6" stopIfTrue="1" operator="equal">
+      <formula>"中級"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="7" stopIfTrue="1" operator="equal">
       <formula>"初級"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="53" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="8" stopIfTrue="1" operator="equal">
       <formula>"中級"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="54" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="9" stopIfTrue="1" operator="equal">
       <formula>"高級"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:H3">
-    <cfRule type="cellIs" dxfId="14" priority="46" stopIfTrue="1" operator="equal">
-      <formula>"中級"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="47" stopIfTrue="1" operator="equal">
-      <formula>"高級"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="48" stopIfTrue="1" operator="equal">
-      <formula>"中級"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I3">
-    <cfRule type="cellIs" dxfId="11" priority="25" stopIfTrue="1" operator="equal">
-      <formula>"初級"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="26" stopIfTrue="1" operator="equal">
-      <formula>"中級"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="27" stopIfTrue="1" operator="equal">
-      <formula>"高級"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G4:H4">
-    <cfRule type="cellIs" dxfId="8" priority="7" stopIfTrue="1" operator="equal">
-      <formula>"初級"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="8" stopIfTrue="1" operator="equal">
-      <formula>"中級"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="9" stopIfTrue="1" operator="equal">
-      <formula>"高級"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G4:H4">
-    <cfRule type="cellIs" dxfId="5" priority="4" stopIfTrue="1" operator="equal">
-      <formula>"中級"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="5" stopIfTrue="1" operator="equal">
-      <formula>"高級"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="6" stopIfTrue="1" operator="equal">
-      <formula>"中級"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I4">
+  <conditionalFormatting sqref="I3:I4">
     <cfRule type="cellIs" dxfId="2" priority="1" stopIfTrue="1" operator="equal">
       <formula>"初級"</formula>
     </cfRule>
@@ -2629,7 +2487,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2684,7 +2542,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="工作表2"/>
   <dimension ref="A1:I1"/>
   <sheetViews>
@@ -2741,7 +2599,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2796,7 +2654,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="工作表3"/>
   <dimension ref="A1:I1"/>
   <sheetViews>
@@ -2853,7 +2711,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2908,14 +2766,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr codeName="工作表4">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.2"/>
@@ -2927,7 +2785,7 @@
     <col min="5" max="5" width="16.109375" style="9" customWidth="1"/>
     <col min="6" max="6" width="14.77734375" style="9" customWidth="1"/>
     <col min="7" max="8" width="12.88671875" style="9" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" style="14" customWidth="1"/>
+    <col min="9" max="9" width="28.44140625" style="33" customWidth="1"/>
     <col min="10" max="10" width="9" style="8"/>
     <col min="11" max="16384" width="9" style="9"/>
   </cols>
@@ -2983,7 +2841,7 @@
       <c r="F3" s="10"/>
       <c r="G3" s="11"/>
       <c r="H3" s="11"/>
-      <c r="I3" s="12"/>
+      <c r="I3" s="32"/>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="10"/>
@@ -2994,76 +2852,41 @@
       <c r="F4" s="10"/>
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
-      <c r="I4" s="12"/>
+      <c r="I4" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:I1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="G3:H3">
-    <cfRule type="cellIs" dxfId="59" priority="16" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="G3:H4">
+    <cfRule type="cellIs" dxfId="41" priority="4" stopIfTrue="1" operator="equal">
+      <formula>"中級"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="40" priority="5" stopIfTrue="1" operator="equal">
+      <formula>"高級"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="39" priority="6" stopIfTrue="1" operator="equal">
+      <formula>"中級"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="7" stopIfTrue="1" operator="equal">
       <formula>"初級"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="17" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="8" stopIfTrue="1" operator="equal">
       <formula>"中級"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="18" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="9" stopIfTrue="1" operator="equal">
       <formula>"高級"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:H3">
-    <cfRule type="cellIs" dxfId="56" priority="13" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="I3:I4">
+    <cfRule type="cellIs" dxfId="35" priority="1" stopIfTrue="1" operator="equal">
+      <formula>"初級"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="2" stopIfTrue="1" operator="equal">
       <formula>"中級"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="14" stopIfTrue="1" operator="equal">
-      <formula>"高級"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="15" stopIfTrue="1" operator="equal">
-      <formula>"中級"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I3">
-    <cfRule type="cellIs" dxfId="53" priority="10" stopIfTrue="1" operator="equal">
-      <formula>"初級"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="11" stopIfTrue="1" operator="equal">
-      <formula>"中級"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="12" stopIfTrue="1" operator="equal">
-      <formula>"高級"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G4:H4">
-    <cfRule type="cellIs" dxfId="50" priority="7" stopIfTrue="1" operator="equal">
-      <formula>"初級"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="8" stopIfTrue="1" operator="equal">
-      <formula>"中級"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="9" stopIfTrue="1" operator="equal">
-      <formula>"高級"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G4:H4">
-    <cfRule type="cellIs" dxfId="47" priority="4" stopIfTrue="1" operator="equal">
-      <formula>"中級"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="5" stopIfTrue="1" operator="equal">
-      <formula>"高級"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="6" stopIfTrue="1" operator="equal">
-      <formula>"中級"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" dxfId="44" priority="1" stopIfTrue="1" operator="equal">
-      <formula>"初級"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="2" stopIfTrue="1" operator="equal">
-      <formula>"中級"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="3" stopIfTrue="1" operator="equal">
       <formula>"高級"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3077,7 +2900,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr codeName="Sheet6">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -3109,38 +2932,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="24"/>
-      <c r="O1" s="24"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
     </row>
     <row r="2" spans="1:15" ht="16.5" customHeight="1">
-      <c r="A2" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="29" t="s">
+      <c r="A2" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="30" t="s">
+      <c r="E2" s="31" t="s">
         <v>27</v>
       </c>
       <c r="F2" s="25" t="s">
@@ -3159,19 +2982,19 @@
         <v>19</v>
       </c>
       <c r="M2" s="25"/>
-      <c r="N2" s="28" t="s">
+      <c r="N2" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="O2" s="27" t="s">
+      <c r="O2" s="29" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:15" s="2" customFormat="1">
-      <c r="A3" s="29"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
+      <c r="A3" s="30"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
       <c r="F3" s="16" t="s">
         <v>22</v>
       </c>
@@ -3196,8 +3019,8 @@
       <c r="M3" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="N3" s="28"/>
-      <c r="O3" s="28"/>
+      <c r="N3" s="24"/>
+      <c r="O3" s="24"/>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" s="17"/>
@@ -3217,13 +3040,13 @@
       <c r="O4" s="18"/>
     </row>
     <row r="5" spans="1:15">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
       <c r="F5" s="21">
         <f t="shared" ref="F5:K5" si="0">SUM(F4:F4)</f>
         <v>0</v>
@@ -3260,23 +3083,23 @@
       <c r="O5" s="22"/>
     </row>
     <row r="6" spans="1:15">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
       <c r="F6" s="25">
         <f>SUBTOTAL(3,$C4:$C4)</f>
         <v>0</v>
       </c>
       <c r="G6" s="25"/>
-      <c r="H6" s="31">
+      <c r="H6" s="27">
         <f>SUBTOTAL(3,$C4:$C4)</f>
         <v>0</v>
       </c>
-      <c r="I6" s="31"/>
+      <c r="I6" s="27"/>
       <c r="J6" s="25">
         <f>SUBTOTAL(3,$C4:$C4)</f>
         <v>0</v>
@@ -3291,13 +3114,13 @@
       <c r="O6" s="22"/>
     </row>
     <row r="7" spans="1:15">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
       <c r="F7" s="25">
         <f>COUNTIF(F4:F4,"&lt;&gt;0")</f>
         <v>1</v>
@@ -3322,13 +3145,13 @@
       <c r="O7" s="25"/>
     </row>
     <row r="8" spans="1:15">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
       <c r="F8" s="26" t="e">
         <f>F7/F6</f>
         <v>#DIV/0!</v>
@@ -3354,20 +3177,6 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="J7:K7"/>
     <mergeCell ref="A1:O1"/>
     <mergeCell ref="N8:O8"/>
     <mergeCell ref="J8:K8"/>
@@ -3384,27 +3193,41 @@
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="H8:I8"/>
     <mergeCell ref="A7:E7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="E4">
+    <cfRule type="cellIs" dxfId="32" priority="4" stopIfTrue="1" operator="equal">
+      <formula>"初級"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="31" priority="5" stopIfTrue="1" operator="equal">
+      <formula>"中級"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="6" stopIfTrue="1" operator="equal">
+      <formula>"高級"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="O4">
-    <cfRule type="cellIs" dxfId="41" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="1" stopIfTrue="1" operator="equal">
       <formula>"初級"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="2" stopIfTrue="1" operator="equal">
       <formula>"中級"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="3" stopIfTrue="1" operator="equal">
-      <formula>"高級"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E4">
-    <cfRule type="cellIs" dxfId="38" priority="4" stopIfTrue="1" operator="equal">
-      <formula>"初級"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="5" stopIfTrue="1" operator="equal">
-      <formula>"中級"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="3" stopIfTrue="1" operator="equal">
       <formula>"高級"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3416,7 +3239,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr codeName="Sheet7">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -3448,38 +3271,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="24"/>
-      <c r="O1" s="24"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
     </row>
     <row r="2" spans="1:15" ht="16.5" customHeight="1">
-      <c r="A2" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="29" t="s">
+      <c r="A2" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="30" t="s">
+      <c r="E2" s="31" t="s">
         <v>27</v>
       </c>
       <c r="F2" s="25" t="s">
@@ -3498,19 +3321,19 @@
         <v>7</v>
       </c>
       <c r="M2" s="25"/>
-      <c r="N2" s="28" t="s">
+      <c r="N2" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="O2" s="27" t="s">
+      <c r="O2" s="29" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:15" s="2" customFormat="1">
-      <c r="A3" s="29"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
+      <c r="A3" s="30"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
       <c r="F3" s="16" t="s">
         <v>11</v>
       </c>
@@ -3535,8 +3358,8 @@
       <c r="M3" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="28"/>
-      <c r="O3" s="28"/>
+      <c r="N3" s="24"/>
+      <c r="O3" s="24"/>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" s="17"/>
@@ -3556,13 +3379,13 @@
       <c r="O4" s="18"/>
     </row>
     <row r="5" spans="1:15">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
       <c r="F5" s="21">
         <f t="shared" ref="F5:K5" si="0">SUM(F4:F4)</f>
         <v>0</v>
@@ -3599,23 +3422,23 @@
       <c r="O5" s="22"/>
     </row>
     <row r="6" spans="1:15">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
       <c r="F6" s="25">
         <f>SUBTOTAL(3,$C4:$C4)</f>
         <v>0</v>
       </c>
       <c r="G6" s="25"/>
-      <c r="H6" s="31">
+      <c r="H6" s="27">
         <f>SUBTOTAL(3,$C4:$C4)</f>
         <v>0</v>
       </c>
-      <c r="I6" s="31"/>
+      <c r="I6" s="27"/>
       <c r="J6" s="25">
         <f>SUBTOTAL(3,$C4:$C4)</f>
         <v>0</v>
@@ -3630,13 +3453,13 @@
       <c r="O6" s="22"/>
     </row>
     <row r="7" spans="1:15">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
       <c r="F7" s="25">
         <f>COUNTIF(F4:F4,"&lt;&gt;0")</f>
         <v>1</v>
@@ -3661,13 +3484,13 @@
       <c r="O7" s="25"/>
     </row>
     <row r="8" spans="1:15">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
       <c r="F8" s="26" t="e">
         <f>F7/F6</f>
         <v>#DIV/0!</v>
@@ -3693,23 +3516,6 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="A1:O1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="O2:O3"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
     <mergeCell ref="L6:M6"/>
     <mergeCell ref="N8:O8"/>
     <mergeCell ref="A7:E7"/>
@@ -3723,27 +3529,44 @@
     <mergeCell ref="H8:I8"/>
     <mergeCell ref="J8:K8"/>
     <mergeCell ref="L8:M8"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="O2:O3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="E4">
+    <cfRule type="cellIs" dxfId="26" priority="4" stopIfTrue="1" operator="equal">
+      <formula>"初級"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="5" stopIfTrue="1" operator="equal">
+      <formula>"中級"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="6" stopIfTrue="1" operator="equal">
+      <formula>"高級"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="O4">
-    <cfRule type="cellIs" dxfId="35" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="1" stopIfTrue="1" operator="equal">
       <formula>"初級"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="2" stopIfTrue="1" operator="equal">
       <formula>"中級"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="3" stopIfTrue="1" operator="equal">
-      <formula>"高級"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E4">
-    <cfRule type="cellIs" dxfId="32" priority="4" stopIfTrue="1" operator="equal">
-      <formula>"初級"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="5" stopIfTrue="1" operator="equal">
-      <formula>"中級"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="3" stopIfTrue="1" operator="equal">
       <formula>"高級"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>